<commit_message>
The OYCIIA full July 2023 iGEM submission
</commit_message>
<xml_diff>
--- a/Open-Yeast-Collection-IIA-new-parts.xlsx
+++ b/Open-Yeast-Collection-IIA-new-parts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rover/Sync/GitHub/Open-Yeast-Collection-IIA-new-parts-package/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C4068A-2877-4F4E-A8B9-234C1F6B7E84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD70E66-C5BA-614D-831F-AF47EA2B0930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27900" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25400" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7638" uniqueCount="7556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7833" uniqueCount="7613">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22704,24 +22704,6 @@
     <t>Yarrowia lipolytica</t>
   </si>
   <si>
-    <t>yh_tGuo-part</t>
-  </si>
-  <si>
-    <t>yh_tLip2-part</t>
-  </si>
-  <si>
-    <t>yh_tSynth8-part</t>
-  </si>
-  <si>
-    <t>yh_tSynthGuo-part</t>
-  </si>
-  <si>
-    <t>yh_tTEF-part</t>
-  </si>
-  <si>
-    <t>yh_tXPR2-part</t>
-  </si>
-  <si>
     <t>Yarrowia lipolytica terminator for GGA with the Open Yeast Collection</t>
   </si>
   <si>
@@ -22743,9 +22725,6 @@
     <t>ggcGAAGACagGGAGcTTAATTAAcTCTAGAcGGTCTCtGCTTtatataactgtctagaaataaagagtatcatctttcaaaCGCTtGAGACCactagtcgCGCTtcGTCTTCtgatgatctaatgttctagggaccacacctcgaagaggtgcgaaccggattgttagtatgcatatgaacgtGaCCtGtgacttgatgtcagcattgccgcttcactagagaagctttgcagactcgctgaaactccacttgtttgcatctataacccagctaacgctgtttaagcaccgaggcccatttaggaagtg</t>
   </si>
   <si>
-    <t>For Twist synthesis. Flanked as a part with BsaI sites for GGA; The part is flanked with BbsI (pOpen-v3) and PacI/SpeI (SEVA) for cloning clonal fragments from Twist post sysnthesis.</t>
-  </si>
-  <si>
     <t>Yarrowia lipolytica terminator from Guo gene for GGA with the Open Yeast Collection</t>
   </si>
   <si>
@@ -22761,23 +22740,215 @@
     <t>OYC-dropout-suGFP</t>
   </si>
   <si>
-    <t xml:space="preserve">OYC Dropout for receiving vectors. Prefix: AAAA Suffix: CGAA </t>
-  </si>
-  <si>
-    <t>OYC Dropout for receiving vectors. Prefix: AGAC Suffix: ATGA</t>
-  </si>
-  <si>
     <t>ggcGAAGACagGGAGcTTAATTAAcTCTAGAcAAAAtGAGACCctcgagggagTTGACGGCTAGCTCAGTCCTAGGTACAGTGCTAGCgtacTTGTTTAACTTTAAGAAGGAGatatacaATGGTTAGCAAAGGCGAGGCGGTTATCAAGGAGTTTATGCGTTTTAAGGTTCACATGGAGGGTAGCATGAATGGTCACGAGTTCGAGATCGAGGGTGAAGGCGAGGGTCGTCCGTACGAAGGCACCCAGACCGCGAAGCTGAAAGTGACCAAGGGTGGCCCGCTGCCGTTCAGCTGGGACATCCTGAGCCCGCAGTTCATGTATGGCAGCCGTGCGTTTACCAAACACCCGGCGGACATTCCGGATTACTATAAGCAAAGCTTCCCGGAAGGTTTTAAATGGGAGCGTGTTATGAACTTCGAAGATGGTGGCGCGGTGACCGTTACCCAGGACACCAGCCTGGAGGATGGCACCCTGATTTACAAGGTGAAACTGCGTGGCACCAACTTTCCGCCGGATGGTCCGGTTATGCAGAAGAAAACGATGGGTTGGGAAGCGAGCACCGAGCGTCTGTATCCGGAAGATGGCGTGCTGAAGGGTGATATCAAAATGGCGCTGCGTCTGAAGGACGGTGGCCGTTACCTGGCGGATTTTAAGACCACCTATAAAGCGAAGAAACCGGTGCAAATGCCGGGTGCGTACAACGTTGACCGTAAACTGGATATTACCAGCCACAACGAGGATTATACCGTGGTTGAGCAATATGAGCGTAGCGAGGGTCGCCACAGCACCGGCGGCATGGACGAACTGTATAAGGGATCCTGActtctgactgagttgcacgctcaattgGGTCTCtCGAAactagtcgCGCTtcGTCTTCtga</t>
   </si>
   <si>
     <t>ggcGAAGACagGGAGcTTAATTAAcTCTAGAcAGACtGAGACCctcgagggagTTGACGGCTAGCTCAGTCCTAGGTACAGTGCTAGCgtacTTGTTTAACTTTAAGAAGGAGatatacaATGGTAGCCCGTAAAGGCGAgGAGCTGTTCACTGGTGTCGTCCCTATTCTGGTGGAACTGGATGGTGATGTCAACGGTCATAAGTTTTCCGTGCGTGGCGAGGGTGAAGGTGACGCAACTAATGGTAAACTGACGCTGAAGTTCATCTGTACTACTGGTAAACTGCCGGTACCTTGGCCGACTCTGGTAACGACGCTGACTTATGGTGTTCAGTGCTTTGCTCGTTATCCGGACCATATGAAGCAGCATGACTTCTTCAAGTCCGCCATGCCGGAAGGCTATGTGCAGGAACGCACGATTTCCTTTAAGGATGACGGCACGTACAAAACGCGTGCGGAAGTGAAATTTGAAGGCGATACCCTGGTAAACCGCATTGAGCTGAAAGGCATTGACTTTAAAGAAGATGGCAATATCCTGGGCCATAAGCTGGAATACAATTTTAACAGCCACAATGTTTACATCACCGCCGATAAACAAAAAAATGGCATTAAAGCGAATTTTAAAATTCGCCACAACGTGGAGGATGGCAGCGTGCAGCTGGCTGATCACTACCAGCAAAACACTCCAATCGGTGATGGTCCTGTTCTGCTGCCAGACAATCACTATCTGAGCACGCAAAGCGTTCTGTCTAAAGATCCGAACGAGAAACGCGATCATATGGTTCTGCTGGAGTTCGTAACCGCAGCGGGCATCACGCATGGTATGGATGAACTGTACAAAGGTTCGTAActtctgactgagttgcacgctcaattgGGTCTCtATGAactagtcgCGCTtcGTCTTCtga</t>
+  </si>
+  <si>
+    <t>yl_tGuo-part</t>
+  </si>
+  <si>
+    <t>yl_tLip2-part</t>
+  </si>
+  <si>
+    <t>yl_tSynth8-part</t>
+  </si>
+  <si>
+    <t>yl_tSynthGuo-part</t>
+  </si>
+  <si>
+    <t>yl_tTEF-part</t>
+  </si>
+  <si>
+    <t>yl_tXPR2-part</t>
+  </si>
+  <si>
+    <t>yl_pTEF_274-part</t>
+  </si>
+  <si>
+    <t>yl_UAS1B-part</t>
+  </si>
+  <si>
+    <t>Yarrowia lipolytica promoter for GGA with the Open Yeast Collection</t>
+  </si>
+  <si>
+    <t>Yarrowia lipolytica UAS (yeast enhancer) for GGA with the Open Yeast Collection</t>
+  </si>
+  <si>
+    <t>ggcGAAGACagGGAGcTTAATTAAcTCTAGAcGGTCTCtGGAGtGAGACGctcgagGTGCACcaattgCGTCTCgTAACctgaggtgtctcacaagtgccgtgcagtcccgcccccacttgcttctctttgtgtgtagtgtacgtacattatcgTgaccgttgttcccgcccacctcgatccggTAACtGAGACCactagtcgCGCTtcGTCTTCtgactatagtgtaacgcaggttcgtctgccctagtctctgacctcgacgggcacgatgatacggactgctaggtagaggctagttacgccctgcc</t>
+  </si>
+  <si>
+    <t>CE_yl_ScRAD52</t>
+  </si>
+  <si>
+    <t>ggcGAAGACagGGAGcTTAATTAAcTCTAGAcGGTCTCcAATGaacgaaattatggatatggacgagaagaaacccgtgttcggcaaccattccgaggacatccagaccaagctggacaagaaactgggccccgaatacatctccaagagagtgggcttcggcacttcccgaatcgcctacatcgagggctggcgagtcattaatctcgctaaccaaatcttcggctacaacggctggtccaccgaggtcaagtccgtcgtcatcgattttttagacgagcgacaaggcaaattttctattggctgcaccgctatcgtgcgagtcactctgacctctggcacctaccgagaagatatcggatacggcaccgtcgagaacgaaagacgaaagcccgctgctttcgagcgagctaagaagtccgctgtgaccgatgctttaaagagatctctgcgaggctttggcaacgctctgggaaactgtctctacgataaggactttctggccaagatcgacaaggtcaagttcgacccccccgatttcgacgagaataatttattccgacctaccgatgagatctccgaatcctcccgaactaacactttacacgagaaccaagaacagcagcagtaccctaacaagcgacgacaactgaccaaggtgaccaacaccaaccccgactccaccaaaaatctggtcaagattgagaacaccgtgtccagaggcactcctatgatggccgcccccgccgaagccaactccaagaactcctctaacaaagacaccgatttaaagtctctcgacgcctccaagcaagatcaagatgatttactggacgactctctgatgttctccgatgacttccaagatgacgacctcatcaatatgggcaacaccaactctaacgttttaaccaccgagaaggaccccgttgtggccaagcagtctcccactgcttcctctaaccccgaggccgagcaaatcacctttgtcaccgccaaggccgccacctctgtccagaacgagcgatacatcggcgaggagtccatttttgaccccaagtaccaagctcagtctatccgacacaccgtcgaccagaccacttccaagcatatccccgcctctgtgctcaaggataaaaccatgaccaccgcccgagactccgtgtacgagaagtttgcccccaagggaaagcagctctccatgaaaaataacgacaaggaactgggccctcacatgctggagggagccggcaaccaagttcctcgagaAaccacccccattaagaccaacgctaccgctttcccccccgctgctgctcccagatttgcccctccctccaaggtggtgcaccccaacggcaacggagccgtgcccgctgtgcctcagcagcgatccactcgacgagaagtgggacgacccaagattaaccccctccatgccagaaagcccacctaaGCTTcGAGACCactagtcgCGCTtcGTCTTCtga</t>
+  </si>
+  <si>
+    <t>ggcGAAGACagGGAGcTTAATTAAcTCTAGAcGGTCTCtTAACttcccacacttgccgttaagggcgtagggtactgcagtctggaatctacgcttgttcagactttgttctagtttctttgtctggccatccgggtaacccatgccggacgcaaaatagactactgaaaatttttttgctttgtggttgggactttagccaagggtataaaagaccaccgtccccgaattacctttcctcttcttttctctctctccttgtcaactcacacccgaaatcgttaagcatttccttctgagtataagaatcattcaaaTACTtGAGACCactagtcgCGCTtcGTCTTCtga</t>
+  </si>
+  <si>
+    <t>ScRAD52 codon optimized for Yarrowia lipolytica as a CE part. Permits improved homologous recombination efficiency of Yarrowia lipolytica.</t>
+  </si>
+  <si>
+    <t>CE_bsaiM1</t>
+  </si>
+  <si>
+    <t>CE_bsaiM2</t>
+  </si>
+  <si>
+    <t>CE_bsaiR</t>
+  </si>
+  <si>
+    <t>AY453694</t>
+  </si>
+  <si>
+    <t>Geobacillus stearothermophilus</t>
+  </si>
+  <si>
+    <t>ggcGAAGACagGGAGcTTAATTAAcTCTAGAcGGTCTCcAATGggaaaaaaagcggaatatggccagggacatccaatctttctggaatatgcggaacagataatccaacataaagaataccaaggtatgccagacctgcgctaccctgatggccgtattcagtgggaagcaccgtcaaatcgtaagagcggtatctttaaggacactaacattaagcgacgtaagtggtgggaacaaaaagcgatttcgatcgggatcgacccgtctagcaaccagtggattagtaagaccgccaaactgattcatcccaccatgcgcaaaccgtgcaaaaagtgcggacgcatcatggatctgcgttatagctatccgaccaaaaacctgattaaacgcattcgcaaactgccgtatgtagatgaatcgttcgaaattgactcactcgaacatattttaaaacttattaaacgtctggtgctccagtatggtgataaagtatacgatgacttgcctaaactactaacgtgcaaggccgtgaaaaatattccgcgcttgggcaacgacctggatacgtggctgaattggattgattctgtttatattccgagtgaacctagcatgctttcgccgggcgctatggcaaatccgccggatcgtctggatgggttccactcattaaatgagtgctgtcggagccatgctgatcgcggtcgttgggaaaaaaacctgcggtcctataccacagatcgccgtgcctttgaatactgggtggacggcgattgggtggcggcggacaagcttatgggcctcatacgcacgaatgaacagatcaagaaggaaacctgcttaaacgataaccacccgggcccgtgttcggcagaccatattggtcctatttcccttggttttgtgcacaggcccgagttccagttgctgtgtaactcatgtaacagcgccaaaaataaccgaatgaccttttcagacgtccaacacttaatcaatgcggagaataatggcgaagaggtggcgtcgtggtactgcaaacacatctgggatctgcgtaagcacgatgttaaaaacaacgaaaacgcactgcgcctgagcaaaattctgcgtgataatcgccatacggctatgttcatcttaagtgagctgctgaaagataatcactatcttttcctgtccacctttctgggcctgcagtatgcagaacgctctgtaagcttttccaatattaaaattgaaaatcatattatcaccggtcagatttcggaacaaccgcgtgatacaaaatacactgaggaacagaaagcccgtcgcatgcgcattggcttcgaggccctgaaaagctatattgagaaagagaacagaaatgccttattagtcatcaacgataaaattattgataaaattaacgaaataaagaatatcttgcaagatattcccgacgaatacaaactgctgaacgaaaaaatctctgagcagttcaacagcgaggaagttagtgatgaactactccgcgatctggttactcatctcccaacgaaagaaagtgaaccagccaactttaaattggcgcgaaaatacttgcaggaaatcatggagatcgtgggggatgaacttagcaaaatgtgggaagatgagcgctacgtccgtcagacctttgcggacttagactaaGCTTcGAGACCactagtcgCGCTtcGTCTTCtga</t>
+  </si>
+  <si>
+    <t>ggcGAAGACagGGAGcTTAATTAAcTCTAGAcGGTCTCcAATGagtaacgcgaaaagcttctcgcttaacgaaaaaaccgaagccaatgcgcttatagatttcattattgaaaaatcgaaccaaagtaaagacttaggttattggctacagaaatcaaaaggccagttttatacccacaatttcattggcgaaaaactggtgacagaaatagtcgaaaacattaaatttaacgatgactcagaagttatcaaaatcatcgacccgttttgcggagatggccgcctgatctgcattttgctggataaatttaatgccattaacaaattccgcaataccttgctcgagattgaattttgggatattgaccccgaagctgtggaagttgcgtacaccaacatcaaggagaaagccaatgcacttgaatttaacgtacagctcaaggggcgtgtatgcgatacctttctgtttgctcaggactactttggctcctatgatatctgcattacaaacccgccatgggtgattatcaaaccggacaaaaaggaaaaggaacgcctgagcaaggaagaagagatcgagtatattgaaattttaaagaatttcgatgacttcttgagtcgttactacccgacgagccttcctaccaaaaaatacggaggatggggcacgaacctggcgcgctgtggtacagaagtggcgctgcgcctgatttccaaagtagggatttgtggtatcgtgtcaccagcatcgctgctgggtgaccaggtcagcgataaccttcgcgtgtggatgttcaataactacgaggtttactcgatttcttacttcgttgcagaagccaaattattcggcaaagtggatcaggccgttattacgctgactttaagccctaagtgtgatgatagcagtggtgatattattccgcatctgttttactacgatcgagagctgtttgaaaaacgttattatatggatgaatatgattggcgtattattaagagcctcaactacgtgattccgattcaatttggtctggagataatcaagatgaatcgtttatttaaaagtctgcctactttaggcgacctggagaacgaaaaagaaggcatttggctaggccgtgaactcgatgaaaccggtatcaaggaaaaattggcgaacaaaggccagtatcgttttatcaaaggtaaaatggtaggccgctacaacctgattgaagagagcaatcagtatattgatgttcgtaaaatagataaaatccccaaatcggtcgaattttaccgtttggtctggcgcgatgtctcccggacgactcaaaaacgccgcctgatctcaaccatcattccgccgaaatatattacgggcaattcgctgaatgtagcgtatttcaaagataataacctgaagaaactgaaagccctgcttgcgatcatgaattcatttgtgttcgaggcgcaagtccgagctaatctgtctaccaaccatatttctttgggcatcattcgcagggcacacattccgaagttagaaggtcgggttgtggacgagcttagccagctcgtggacaattatgttaacgaggaaagcgaattactactggaggtaaaagtggccaaagcatatgggctctcatttgaggatttcagcagcattctgtctttgttcgacaagattggcaaagacgaaaaagaaaagatcctgcaggtggccaaaaaatatttaaaggggggaatcaaaaatgattcctaaGCTTcGAGACCactagtcgCGCTtcGTCTTCtga</t>
+  </si>
+  <si>
+    <t>ggcGAAGACagGGAGcTTAATTAAcTCTAGAcGGTCTCcAATGatgctgatcattaagcacgtacctccgggcggcaactggaaggacattccggagtgggtcccttcgaaacgcttagagcaaattcgaaaaagctatgcagaaggcaagggcagccgttctacgtattacggtcgcctgctgccagacatgccgagctatacaatcaacacctatttcaatcgcccgggaaacggttgtcatattcattacgagcaggataggaccctgtcgcagcgtgaggcggcgcgccttcagagctttcctgacgattttattttttatggaagcaaaaccgccattaacaatcagattggcaatgccgtaccgccgctgctggcgtatcagatagcgaaagcattcccctttaaaggacagttcgtcgacctgttcagtggcgccggcggtctttcgctaggctttttatgggcaggttggaaacctattattgccaacgatattgataaatgggcactcaccacgtacatgaataacatccacaatgaagttgttctgggggatattcgggatgaaaaagtgtccgaaaccatcattcaaaaatgcctcatcgcgaagaaaagcaaccccgatcgcccattgttcgttctgggtggacccccgtgccagggcttctcgactgcgggcaaaaagcgtagcattgtcgatgaacgcaactggctgtttgaatcttacgtgtccatactgaaagaagttaaaccggatggctttattttcgaaaatgtcaccggtttgctgagtatggaaaaaggggcgtttttcgaaatggtgaagtcagaactgagcaaaactgtgtctaacctctttgtgtataaactaaatagtgtggattatggggttccacagcgccgtaatcgtgtagtaatcatcggtgactcaacgggtacgaaaaacagcgaaccgccaattccgattacatcattaaaaggcgagaaaaccttatttgatgccctttcctcagccatctcagtgaaagaagctctgtctgacctgccgttgctttccccgaatgaagatggctcgtggaaaaactacgtgtgtgagccgcagaatatctaccagagctttatgcgtaagaagattactgctcaacaatacattgaaatgttgagcagtttagcgatcatctaaGCTTcGAGACCactagtcgCGCTtcGTCTTCtga</t>
+  </si>
+  <si>
+    <t>Geobacillus stearothermophilus bsaIR restriction Endonuclease codon optimized for E. coli, defined as a CE (AATG/GCTT) part.</t>
+  </si>
+  <si>
+    <t>Geobacillus stearothermophilus bsaiM1 methylase codon optimized for E. coli, defined as a CE (AATG/GCTT) part.</t>
+  </si>
+  <si>
+    <t>Geobacillus stearothermophilus bsaiM2 methylase codon optimized for E. coli, defined as a CE (AATG/GCTT) part.</t>
+  </si>
+  <si>
+    <t>BC_His_TEVcut</t>
+  </si>
+  <si>
+    <t>BC_pre_Ost1_pro_αMF_I_His_TEVcut</t>
+  </si>
+  <si>
+    <t>BC_Wci_αMF_signal_His_tag_TEVcut</t>
+  </si>
+  <si>
+    <t>BT1_alpha_amylase_signal</t>
+  </si>
+  <si>
+    <t>BT1_glucoamylase_signal</t>
+  </si>
+  <si>
+    <t>BT1_inulinase_signal</t>
+  </si>
+  <si>
+    <t>BT1_invertase_signal</t>
+  </si>
+  <si>
+    <t>BT1_killer_protein_signal</t>
+  </si>
+  <si>
+    <t>ggcGAAGACagGGAGcTTAATTAAcTCTAGAcGGTCTCcTACTatgggatcttctcatcaccatcatcatcattcctctggaggagagaacttgtattttcagggtggAATGaGAGACCactagtcaCGCTtcGTCTTCtgagagaggccctacaaggaaatagcgtactttagttcggacgcccagtgttcacaaggacaccgccccagatcgtactatcatgtattcctgcgatggcctcaataattgccttaccagtgaactgtcactgaatcacctaccgctttcgtgctttactgtaaacaggga</t>
+  </si>
+  <si>
+    <t>ggcGAAGACagGGAGcTTAATTAAcTCTAGAcGGTCTCcTACTatgaggcaggtttggttctcttggattgtgggattgttcctatgttttttcaacgtttcttctgctgctccagtcaacactacaacagaagatgaaacggcacaaattccggctgaagctgtcatcggttactcagatttagaaggggatttcgatgttgctgttttgccattttccaacagcacaaataacgggttattgtttataaatactactattgccagcattgctgctaaagaagaaggggtatctctcgagaaaagagaggctgaagctggacatcaccatcaccatcacggagagaatctgtactttcaaggAATGgGAGACCactagtcgCGCTtcGTCTTCtga</t>
+  </si>
+  <si>
+    <t>ggcGAAGACagGGAGcTTAATTAAcTCTAGAcGGTCTCcTACTatgcaactttctttactaacttctttggccattgtttccactttactaggctcttcgtttgctgctccagtggagaatatcaatatcaaagacaatggcaatggcaccagtgaagctgatgttcctggaacttctcaaggtgttgagtttccgtttgccaaagaagccatcattgaagctgtttctttaggcaatgatattgctccaattgttctcaatgatgctgtttattttgtcaataccaccactgttgacaaagagctggaaagcaaacttggcaaacgaggacatcaccatcaccatcacggagagaatctgtactttcaaggAATGgGAGACCactagtcgCGCTtcGTCTTCtga</t>
+  </si>
+  <si>
+    <t>ggcGAAGACagGGAGcTTAATTAAcTCTAGAcGGTCTCcTACTatggtggcatggtggtccttattcttatatggacttcaagttgctgctcctgcccttgctatgagatttcctagtattttcactgctgtgctatttgccgctagttccgctctagctgctccagttaatactactactgaagatgaattggagggtgacttcgatgttgctgttctgcctttttccgcttctatcgcagccaaggaagaaggtgtatccctagagaagcgttCCATgGAGACCactagtcgCGCTtcGTCTTCtgat</t>
+  </si>
+  <si>
+    <t>ggcGAAGACagGGAGcTTAATTAAcTCTAGAcGGTCTCcTACTatgtctttcagatccctattggcattgtcagggttggtctgttctggattggctatgagatttcctagtattttcactgctgtgctatttgccgctagttccgctctagctgctccagttaatactactactgaagatgaattggagggtgacttcgatgttgctgttctgcctttttccgcttctatcgcagccaaggaagaaggtgtatccctagagaagcgttccatgGAGACCactagtcgCGCTtcGTCTTCtgatacagac</t>
+  </si>
+  <si>
+    <t>ggcGAAGACagGGAGcTTAATTAAcTCTAGAcGGTCTCcTACTatgaaactggcttactccctgttgctacctctggctggagtttccgctatgagatttcctagtattttcactgctgtgctatttgccgctagttccgctctagctgctccagttaatactactactgaagatgaattggagggtgacttcgatgttgctgttctgcctttttccgcttctatcgcagccaaggaagaaggtgtatctctagagaagcgttCCATgGAGACCactgtcttccgCGCTtcGTCTTCtgaggattaaccgatg</t>
+  </si>
+  <si>
+    <t>ggcGAAGACagGGAGcTTAATTAAcTCTAGAcGGTCTCcTACTatgttattgcaagcttttttatttctgctggcaggttttgcagcaaagatttctgccatgagatttcctagtattttcactgctgtgctatttgccgctagttccgctctagctgctccagttaatactactactgaagatgaattggagggtgacttcgatgttgctgttctgcctttttccgcttctatcgcagccaaggaagaaggtgtatccctagagaagcgttCCATgGAGACCactagtcgCGCTtcGTCTTCtgaacgc</t>
+  </si>
+  <si>
+    <t>ggcGAAGACagGGAGcTTAATTAAcTCTAGAcGGTCTCcTACTatgaccaaaccaacgcaagtcttagttcgttcagtctctattttattcttcatcacactgttgcacttggttgttgcaatgagatttcctagtattttcactgctgtgctatttgccgctagttccgctctagctgctccagttaatactactactgaagatgaattggagggtgacttcgatgttgctgttctgcctttttccgcttctatcgcagccaaggaagaaggtgtatccctagagaagcgttCCATgGAGACCactagtcgCGCTtcGTCTTCtga</t>
+  </si>
+  <si>
+    <t>yl_pACL2-part</t>
+  </si>
+  <si>
+    <t>yl_pDGA1-part</t>
+  </si>
+  <si>
+    <t>yl_pGAPDH-part</t>
+  </si>
+  <si>
+    <t>yl_pICL-part</t>
+  </si>
+  <si>
+    <t>yl_pIDH2-part</t>
+  </si>
+  <si>
+    <t>yl_pLIP2-part</t>
+  </si>
+  <si>
+    <t>ggcGAAGACagGGAGcTTAATTAAcTCTAGAcGGTCTCtGGAGaaaatgacgacaattcgaaccgaggccaattgagcacgccgaagcagtttcaacgcaatcggccgcgattcggaccagttgggccgctcttaggcagtcaccaaccagatgttctgcacggatttccccgattgtggaaatgaaatcgacgccggcgtcatggcaatcgacagttgggggagagataaatcggtggtcacgtgtacaccccccacgagcgActcccgtgccactttctccccagcgaccgttatctcaactcacttcccctctctcaacagttaacccaaccctcaaccaaattgacgtggttagcggtttggcaggcgacaagcgaaattgacttttccaacaaactcagcacgccaccacgcccgttcgccatgcatgttgtacccctcaccgaggccaccaggattgggtcaaagtgagggggagtatcaacaagaaggaaaaagggtcttttgggagctccaaaatagttggggaggcggaccaacagagacatatatagactcgaaaccaatgtcacaaatccatctttaccaaataaagttagggacacaaaaccgctctccaaacaggatataattgtcccaccaccaccacacacacacaccacccaacccaacatttagcctccgtctgctacaacttaatcaggcacgactcactcttctttctacgtgacacaaacagagcgacacctacggagcgacacccccctcgaccgacacagaaacagcgtcgatcacacacacacacacacacacaccgaatccgacactcaccagatcaatcTACTtGAGACCactagtcgCGCTtcGTCTTCtga</t>
+  </si>
+  <si>
+    <t>ggcGAAGACagGGAGcTTAATTAAcTCTAGAcGGTCTCtGGAGgatccatcctcgaccagtggcacgctcaaccccatggttcgcttttctcttttcgtctatcctgaactgagtttttttccacgccaactgatatccccttacgttaccccctcatcacctggtgaggcgaaactgtaaggtgaaagctaaaaatgacatctcagctgcacgaaggaccggggcttaaaagacgggctggtgcttgtgatttaaaactggacaaatctcagcttgcttgaaattttggActccaactgtttccgagcgaatcgcacacaaaccgggcttctctctgcagaccacgcccccgaaactctttctcccaccaccaccaacactccctttccattcccacaccgttcctctctcgtgcgtcatccttgcgcaatcatcttcgtctgcgacatattgtacgacatacagtaccacggaacgtttcagaccgtcgacgtgaacacatcttaggaacagcaacctgagctacagaaatctatctataggcggataaaaaaacgcacccactgctcgtcctccttgctcctcgaaaccgactcctctacacacgtcaaatccgaggttgaaatcttccccacatttggcagccaaaccagcacatcccagcaacctcgcacagcgccgaaatcgacctgtcgacttggccacaaaaaaaagcaccggctctgcaacagttctcacgaccaattacgtacaagtacgaaatcgttcgtggaccgtgactgataagctcccactttttcttctaacaacaggcaacagacaagtcacacaaaacaaaagctTACTtGAGACCactagtcgCGCTtcGTCTTCtga</t>
+  </si>
+  <si>
+    <t>ggcGAAGACagGGAGcTTAATTAAcTCTAGAcGGTCTCtGGAGtaccaaccacagattacgacccattcgcagtcacagttcactagggtttgggttgcatccgttgagagtggtttgtttttaaccttctccatgtgctcactcaggttttgggttcagatcaaatcaaggcgtgaaccactgtttgaggacaaatgtgacacaaccaaccagtgtcaggggcaagtccgtgacaaaggggaagatacaatgcaattactgacagttacggactgcctcgatgccctaaccttgccccaaaataagacaactgtcctcgtttaagcgcaaccctattcagcgtcacgtcataatagcgtttggatagcactagActatgaggagcgttttatgttgcggtgagggcgattggtgctcatatgggAtcaattgaggtggtggaacgagcttagtctAcaattgaggtgcgagcgacacaattgggtgtcacgtggcctaattgacctcggatcgtggagtccccagttatacagcaaccacgaggtgcatgagtaggTgacgtcaccagacaatagggtttttttggactggagagggtagggcaaaagcgctcaacgggctgtttggggagctatgggggaggaattggcgatatttgtgaggttgacggctccgatttgcgtgttttgtcgcttctgcatctccccatacccatatcttccctccccacctctttccacgataattttacggatcagcaataaggttccttctcctagtttccacgtccatatatatctatgctgcgtcgtccttttcgtgacatcaccaaaacacatacaaaaTACTtGAGACCactagtcgCGCTtcGTCTTCtga</t>
+  </si>
+  <si>
+    <t>ggcGAAGACagGGAGcTTAATTAAcTCTAGAcGGTCTCtGGAGgaccccctccttttgccagtatatccaccgcaacacccaccatgagcgacatctgataccgtgccgcgaccactaccccaaataagctccaactaatatgccgaggcaggtgggaaactatgcactccagttgacgctgtagaagcacatggaaggtgcggaggcggtggcaacgaggggcatgagccatcaacgagtaaccacagacaaggcaaggggggaaacgcgaccggaatctctcgcggtcacgtgacccgcccgggttccactcgtccatgttgtgtctctggtgActtcggccgactcgcattggttaaacttccaccaccgcaatcacgtcccactggccaaactttttctgctttctctgactttttctggccaaaaggcaacgtcggaaagggtcgggaggattcggaaccgacgaaaatcggccggctccagcgggggtagttcggcagtcctggtgggagctctaggggagctgtggtctgtgtagggcgcgggtccgggtttgttgggtgtcaaatcacgtgtttttgcccccccgctgagccggactccgacaaccgtgtctccaacggcctgactaagctgctcccagcactctgccgtagcgttggtctgtcctgtcgcactctgttcaaagacagaagaaagaaaaagctaacctccacgtcagagacaatggtagaaggcttgttccttgcaaccgaggagagtgagtgttctcggcacgagcatcatgggcgatctggagggtatttttgaggggaaaaaacgggatcaggacaaacagaggccacagaccgggaatctgggccccaaaacggccttttcccgtcgcaaaaccggtctacatacaccccttcggcccgccacaggccggtgtgaaaaaccctaaagcttgcttcaaaccagacggacgcacagcaagacacatcatgaagagtcacctgcagtatatatagatctggggatccccagtagactgaccaagcatacaaaTACTtGAGACCactagtcgCGCTtcGTCTTCtga</t>
+  </si>
+  <si>
+    <t>ggcGAAGACagGGAGcTTAATTAAcTCTAGAcGGTCTCtGGAGagtacaattgtgctgtgcggatgtccatgagaaagttggtacttgcgActctcccattgctccatgtttcgccctgtttttcacagctcctttggaccttgtattcctgcgatcaaacagcgtatgaagctaaaattgcgtttttcggTgacgattggctcggacttaagagggagctgtgggagaggacttggaagggcgatagagggagcgattggacgggctttacagggttagggatccgtatcattgattttacgggccaaacccttccaccgcctttcctgtcgctccccaaccccccaattgaacccgttatccagcttaacatatagttacatattcctcagactttggcgtacattcatcttttttgccagtgcagcttttttgcagtgccagttgcatattgtttatccgggggatgaggggagttagacggacgtgggtaggggtaggggtttaggggaccgaacaggagccctcggatatacatggggatgccaagcatagcaattcccggtcaatccggacaccctagccccaataatgagccctccaggagctccagacaccagcagtccctcaaaccctattggttcttacgcagcaaagtgttggtccatcactacgctcccaacccgtgtgtctttgtgtttttggtgcttgtgtaatgttaattttttttccctttggtcccacgttccctccttccacacactacaccttagcgcgatttactcgtcgacatcacttttttttcttgtcgccaacttcgtggaacccccaaagaaatcacaTACTtGAGACCactagtcgCGCTtcGTCTTCtga</t>
+  </si>
+  <si>
+    <t>ggcGAAGACagGGAGcTTAATTAAcTCTAGAcGGTCTCtGGAGaaacttctccgagtctgtgccttcaggtgggcatagttgatgggtgttttgaagttaatagtggggaagaactatggcaaacaagcagatgcaggcaccttgtaactgcagaccggttcttgtctaccgactccgctgcacctgtgccgcggtacatgtcgtcacaggctgcggggttcggaggcccccttgcaacctcctttgatagttgctatggccccaaagagttatacgagatagacccacagatctacttgactgttgtcacagaacctgctaggtttgcttattgtacccgctttgtagctactgtacaacgacaacgtcaaaaattgTgacgcgaacaaactccagatgcagaacccaaacctctctctcagagtttcgagtgcttctacctcacagtaaagtggaggtggacctgcaagggaattcagtcacaaggccccgaatgtctccgaaactccaatcggaccgtttaaacagactaatatcacgtcattgattgatattagcatccggcaagagccgcaaggttatctcctcaccaatgagcctgttgtacggctcattccgcatctgcggctgattcagtttcgagtggggatggtagacttcattgcagcattcctaaccttctacttggtccgtggagatgtcatggacatcgattttgggctgagaagccttttgacgatgttgatatcactgaccgctaatttactctggcagtttctccggctctcgaggcatcgtcgatcaccaaacactatctgctagtctaaatgtccgacacgacagcttttgatcgccgtgaacggcgcagacctcatgcaccatgcaccagggccaaatcaattacgggtcgcttagcgttgcagtcggggcattatggtggaagttccgatacggcacagacacattccatagtggggggattggattataaaagggccatagaaagccctcaattgatacccaagtaccagctctcctcactTACTtGAGACCactagtcgCGCTtcGTCTTCtga</t>
+  </si>
+  <si>
+    <t>Komagataella phaffii (Pichia pastoris)</t>
+  </si>
+  <si>
+    <t>https://freegenes.github.io/genes/BBF10K_003419.html</t>
+  </si>
+  <si>
+    <t>CD_ymScarlet3</t>
+  </si>
+  <si>
+    <t>ggcGAAGACagGGAGcTTAATTAAcTCTAGAcGGTCTCcAATGgactctactgaagctgtgatcaaggagttcatgagattcaaggttcacatggaaggctctatgaacggtcatgaattcgaaatcgagggtgaaggtgaaggtagaccttacgaaggtactcagactgctaagttgagagttaccaagggtggtcctttgcctttttcttgggatatcctgtctcctcagtttatgtacggttccagagccttcactaagcatcctgctgatattcctgactactggaagcagtcttttcctgaaggtttcaagtgggagagagtgatgaactttgaagatggtggtgctgtttctgttgctcaggatacttctctggaagatggtactctgatctacaaggtgaagttgagaggtactaacttccctcctgatggtccTgttatgcagaagaaaactatgggttgggaagcctctactgaaagattgtaccctgaggatgttgttctgaagggtgacattaagatggctctgagattgaaggatggtggtagatacttggctgatttcaagaccacctacagagctaagaagcctgttcagatgcctggtgctttcaacatcgacagaaagttggacatcacttctcataacgaggattacactgtggtggaacagtacgaaagatctgttgctagacactctactggtggttctggtggttctggAGGTcGAGACCactagtcgCGCTtcGTCTTCtga</t>
+  </si>
+  <si>
+    <t>OYC Dropout for for Open Yeast Collection receiving vectors. Fits between assembly connectors (prefix: AGAC, suffix: ATGA). BsaI sites can be independently replaced with overlapping oligos.</t>
+  </si>
+  <si>
+    <t>OYC Dropout for Open Yeast Collection receiving vectors. Fits between the E. coli backbone (prefix: AAAA, suffix: CGAA ). BsaI sites can be independently replaced with overlapping oligos.</t>
+  </si>
+  <si>
+    <t>Brilliant and fast-maturing mScarlet3 codon optimized for Saccharomyces cerevisiae, Komagataella phaffii (Pichia pastoris), Yarrowia lipolytical and likely other yeast.</t>
+  </si>
+  <si>
+    <t>His-tag followed by a TEV protease cleavage site as a BC part in the Yeast Protein Expression Toolkit. Codon optimized for Saccharomyces cerevisiae, Komagataella phaffii (Pichia pastoris), Yarrowia lipolytical and likely other yeast.</t>
+  </si>
+  <si>
+    <t>Yeast α-mating factor secretion signals and endogenous signal peptides for recombinant protein secretion as a BT1 part in the Yeast Protein Expression Toolkit. Codon optimized for Saccharomyces cerevisiae, Komagataella phaffii (Pichia pastoris), Yarrowia lipolytical and likely other yeast.</t>
+  </si>
+  <si>
+    <t>For Twist synthesis. Extension of the Open Yeast Collection. Flanked as a part with BsaI sites for GGA; The part is flanked with BbsI (pOpen-v3) and PacI/SpeI (SEVA) for cloning clonal fragments from Twist post sysnthesis.</t>
+  </si>
+  <si>
+    <t>For Twist synthesis. Extension of the Open Yeast Collection. Flanked as a part with BsaI sites for GGA; The part is flanked with BbsI (pOpen-v3) and PacI/SpeI (SEVA) for cloning clonal fragments from Twist post sysnthesis. Has BsmBI dropout to facilitate recursive assembly of multiple UAS sequences. mScarlet or suGFP selection markers can be clone into the BsmBI dropout to facilitate cloning.</t>
+  </si>
+  <si>
+    <t>For Twist synthesis. Extension of the Open Yeast Collection. Flanked as a part with BsaI sites for GGA; The part is flanked with BbsI (pOpen-v3) and PacI/SpeI (SEVA) for cloning clonal fragments from Twist post sysnthesis. Adapted from E. coli Proetin Expression Toolkit.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -22938,8 +23109,15 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -22956,6 +23134,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFE2EFD9"/>
         <bgColor rgb="FFE2EFD9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -23086,7 +23270,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -23134,11 +23318,27 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -23347,7 +23547,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A14:M40" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A14:M68" headerRowCount="0">
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
@@ -23596,20 +23796,20 @@
   <dimension ref="A1:M963"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="14" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="14" topLeftCell="B27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="G16" sqref="G16"/>
+      <selection pane="bottomRight" activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="33" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
     <col min="8" max="8" width="13.85546875" customWidth="1"/>
     <col min="9" max="9" width="15.5703125" customWidth="1"/>
@@ -23659,12 +23859,12 @@
       <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:13" ht="46" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="39"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="41"/>
+      <c r="A5" s="42"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="44"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -23763,6 +23963,14 @@
       <c r="B11" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="L11" s="40">
+        <f>SUM(L15:L59)</f>
+        <v>19643</v>
+      </c>
+      <c r="M11" s="47">
+        <f>20000-L11</f>
+        <v>357</v>
+      </c>
     </row>
     <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
@@ -23857,19 +24065,19 @@
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="30" t="s">
-        <v>7533</v>
+        <v>7547</v>
       </c>
       <c r="B15" s="30" t="s">
         <v>52</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>7546</v>
+        <v>7610</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>7445</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>7547</v>
+        <v>7540</v>
       </c>
       <c r="F15" s="37" t="s">
         <v>39</v>
@@ -23889,29 +24097,29 @@
       <c r="K15" t="b">
         <v>0</v>
       </c>
-      <c r="L15" s="10">
+      <c r="L15" s="41">
         <f>LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M15,CHAR(160)," ")," ",""))))</f>
         <v>310</v>
       </c>
       <c r="M15" t="s">
-        <v>7545</v>
+        <v>7539</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="30" t="s">
-        <v>7534</v>
+        <v>7548</v>
       </c>
       <c r="B16" s="30" t="s">
         <v>52</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>7546</v>
+        <v>7610</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>7445</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>7548</v>
+        <v>7541</v>
       </c>
       <c r="F16" s="37" t="s">
         <v>7485</v>
@@ -23931,29 +24139,29 @@
       <c r="K16" t="b">
         <v>0</v>
       </c>
-      <c r="L16" s="10">
+      <c r="L16" s="41">
         <f>LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M16,CHAR(160)," ")," ",""))))</f>
         <v>310</v>
       </c>
       <c r="M16" t="s">
-        <v>7540</v>
+        <v>7534</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="30" t="s">
-        <v>7535</v>
+        <v>7549</v>
       </c>
       <c r="B17" s="30" t="s">
         <v>52</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>7546</v>
+        <v>7610</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>7445</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>7549</v>
+        <v>7542</v>
       </c>
       <c r="F17" s="37" t="s">
         <v>7485</v>
@@ -23973,29 +24181,29 @@
       <c r="K17" t="b">
         <v>0</v>
       </c>
-      <c r="L17" s="10">
+      <c r="L17" s="41">
         <f>LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M17,CHAR(160)," ")," ",""))))</f>
         <v>310</v>
       </c>
       <c r="M17" t="s">
-        <v>7541</v>
+        <v>7535</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="30" t="s">
-        <v>7536</v>
+        <v>7550</v>
       </c>
       <c r="B18" s="30" t="s">
         <v>52</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>7546</v>
+        <v>7610</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>7445</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>7539</v>
+        <v>7533</v>
       </c>
       <c r="F18" s="38" t="s">
         <v>7485</v>
@@ -24015,29 +24223,29 @@
       <c r="K18" t="b">
         <v>0</v>
       </c>
-      <c r="L18" s="10">
+      <c r="L18" s="41">
         <f>LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M18,CHAR(160)," ")," ",""))))</f>
         <v>310</v>
       </c>
       <c r="M18" t="s">
-        <v>7542</v>
+        <v>7536</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="30" t="s">
-        <v>7537</v>
+        <v>7551</v>
       </c>
       <c r="B19" s="30" t="s">
         <v>52</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>7546</v>
+        <v>7610</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>7445</v>
       </c>
       <c r="E19" s="30" t="s">
-        <v>7539</v>
+        <v>7533</v>
       </c>
       <c r="F19" s="37" t="s">
         <v>7485</v>
@@ -24057,29 +24265,29 @@
       <c r="K19" t="b">
         <v>0</v>
       </c>
-      <c r="L19" s="10">
-        <f t="shared" ref="L19:L40" si="0">LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M19,CHAR(160)," ")," ",""))))</f>
+      <c r="L19" s="41">
+        <f t="shared" ref="L19:L39" si="0">LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M19,CHAR(160)," ")," ",""))))</f>
         <v>310</v>
       </c>
       <c r="M19" t="s">
-        <v>7543</v>
+        <v>7537</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="30" t="s">
-        <v>7538</v>
+        <v>7552</v>
       </c>
       <c r="B20" s="30" t="s">
         <v>52</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>7546</v>
+        <v>7610</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>7445</v>
       </c>
       <c r="E20" s="30" t="s">
-        <v>7539</v>
+        <v>7533</v>
       </c>
       <c r="F20" s="37" t="s">
         <v>7485</v>
@@ -24099,29 +24307,29 @@
       <c r="K20" t="b">
         <v>0</v>
       </c>
-      <c r="L20" s="10">
+      <c r="L20" s="41">
         <f t="shared" si="0"/>
         <v>310</v>
       </c>
       <c r="M20" t="s">
-        <v>7544</v>
+        <v>7538</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="30" t="s">
-        <v>7550</v>
+        <v>7543</v>
       </c>
       <c r="B21" t="s">
         <v>1683</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>7546</v>
+        <v>7610</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>7445</v>
+        <v>7460</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>7552</v>
+        <v>7606</v>
       </c>
       <c r="F21" s="37" t="s">
         <v>7485</v>
@@ -24141,29 +24349,29 @@
       <c r="K21" t="b">
         <v>0</v>
       </c>
-      <c r="L21" s="10">
+      <c r="L21" s="41">
         <f t="shared" si="0"/>
         <v>886</v>
       </c>
       <c r="M21" t="s">
-        <v>7554</v>
+        <v>7545</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="30" t="s">
-        <v>7551</v>
+        <v>7544</v>
       </c>
       <c r="B22" t="s">
         <v>1683</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>7546</v>
+        <v>7610</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>7445</v>
+        <v>7460</v>
       </c>
       <c r="E22" s="30" t="s">
-        <v>7553</v>
+        <v>7605</v>
       </c>
       <c r="F22" s="37" t="s">
         <v>7485</v>
@@ -24183,339 +24391,1257 @@
       <c r="K22" t="b">
         <v>0</v>
       </c>
-      <c r="L22" s="10">
+      <c r="L22" s="41">
         <f t="shared" si="0"/>
         <v>910</v>
       </c>
       <c r="M22" t="s">
+        <v>7546</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="30" t="s">
+        <v>7553</v>
+      </c>
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>7610</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>7445</v>
+      </c>
+      <c r="E23" s="30" t="s">
         <v>7555</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="30"/>
-      <c r="D23" s="5"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="36"/>
+      <c r="F23" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="36">
+        <v>23053080</v>
+      </c>
+      <c r="H23" t="s">
+        <v>7532</v>
+      </c>
+      <c r="I23" t="s">
+        <v>7532</v>
+      </c>
       <c r="J23" t="b">
         <v>0</v>
       </c>
       <c r="K23" t="b">
         <v>0</v>
       </c>
-      <c r="L23" s="10">
+      <c r="L23" s="41">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>351</v>
+      </c>
+      <c r="M23" t="s">
+        <v>7560</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="30"/>
-      <c r="D24" s="5"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="36"/>
+      <c r="A24" s="30" t="s">
+        <v>7554</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1728</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>7611</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>7460</v>
+      </c>
+      <c r="E24" s="30" t="s">
+        <v>7556</v>
+      </c>
+      <c r="F24" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" s="36">
+        <v>23053080</v>
+      </c>
+      <c r="H24" t="s">
+        <v>7532</v>
+      </c>
+      <c r="I24" t="s">
+        <v>7532</v>
+      </c>
       <c r="J24" t="b">
         <v>0</v>
       </c>
       <c r="K24" t="b">
         <v>0</v>
       </c>
-      <c r="L24" s="10">
+      <c r="L24" s="41">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>310</v>
+      </c>
+      <c r="M24" t="s">
+        <v>7557</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="30"/>
-      <c r="D25" s="5"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="36"/>
+      <c r="A25" s="30" t="s">
+        <v>7589</v>
+      </c>
+      <c r="B25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>7610</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>7445</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7555</v>
+      </c>
+      <c r="F25" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="G25" s="36">
+        <v>29188186</v>
+      </c>
+      <c r="H25" t="s">
+        <v>7532</v>
+      </c>
+      <c r="I25" t="s">
+        <v>7532</v>
+      </c>
       <c r="J25" t="b">
         <v>0</v>
       </c>
       <c r="K25" t="b">
         <v>0</v>
       </c>
-      <c r="L25" s="10">
+      <c r="L25" s="41">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>878</v>
+      </c>
+      <c r="M25" s="30" t="s">
+        <v>7595</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="30"/>
-      <c r="D26" s="5"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="36"/>
+      <c r="A26" s="30" t="s">
+        <v>7590</v>
+      </c>
+      <c r="B26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>7610</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>7445</v>
+      </c>
+      <c r="E26" t="s">
+        <v>7555</v>
+      </c>
+      <c r="F26" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="G26" s="36">
+        <v>29188186</v>
+      </c>
+      <c r="H26" t="s">
+        <v>7532</v>
+      </c>
+      <c r="I26" t="s">
+        <v>7532</v>
+      </c>
       <c r="J26" t="b">
         <v>0</v>
       </c>
       <c r="K26" t="b">
         <v>0</v>
       </c>
-      <c r="L26" s="10">
+      <c r="L26" s="41">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>877</v>
+      </c>
+      <c r="M26" s="30" t="s">
+        <v>7596</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="30"/>
-      <c r="D27" s="5"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="36"/>
+      <c r="A27" s="30" t="s">
+        <v>7591</v>
+      </c>
+      <c r="B27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>7610</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>7445</v>
+      </c>
+      <c r="E27" t="s">
+        <v>7555</v>
+      </c>
+      <c r="F27" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="G27" s="36">
+        <v>29188186</v>
+      </c>
+      <c r="H27" t="s">
+        <v>7532</v>
+      </c>
+      <c r="I27" t="s">
+        <v>7532</v>
+      </c>
       <c r="J27" t="b">
         <v>0</v>
       </c>
       <c r="K27" t="b">
         <v>0</v>
       </c>
-      <c r="L27" s="10">
+      <c r="L27" s="41">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>880</v>
+      </c>
+      <c r="M27" s="30" t="s">
+        <v>7597</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="30"/>
-      <c r="D28" s="5"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="36"/>
+      <c r="A28" s="30" t="s">
+        <v>7592</v>
+      </c>
+      <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="30" t="s">
+        <v>7610</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>7445</v>
+      </c>
+      <c r="E28" t="s">
+        <v>7555</v>
+      </c>
+      <c r="F28" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="G28" s="36">
+        <v>29188186</v>
+      </c>
+      <c r="H28" t="s">
+        <v>7532</v>
+      </c>
+      <c r="I28" t="s">
+        <v>7532</v>
+      </c>
       <c r="J28" t="b">
         <v>0</v>
       </c>
       <c r="K28" t="b">
         <v>0</v>
       </c>
-      <c r="L28" s="10">
+      <c r="L28" s="41">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1085</v>
+      </c>
+      <c r="M28" s="30" t="s">
+        <v>7598</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="30"/>
-      <c r="D29" s="5"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="36"/>
+      <c r="A29" s="30" t="s">
+        <v>7593</v>
+      </c>
+      <c r="B29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="30" t="s">
+        <v>7610</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>7445</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7555</v>
+      </c>
+      <c r="F29" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="G29" s="36">
+        <v>29188186</v>
+      </c>
+      <c r="H29" t="s">
+        <v>7532</v>
+      </c>
+      <c r="I29" t="s">
+        <v>7532</v>
+      </c>
       <c r="J29" t="b">
         <v>0</v>
       </c>
       <c r="K29" t="b">
         <v>0</v>
       </c>
-      <c r="L29" s="10">
+      <c r="L29" s="41">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>877</v>
+      </c>
+      <c r="M29" s="30" t="s">
+        <v>7599</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="30"/>
-      <c r="D30" s="5"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="36"/>
+      <c r="A30" s="30" t="s">
+        <v>7594</v>
+      </c>
+      <c r="B30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>7610</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>7445</v>
+      </c>
+      <c r="E30" t="s">
+        <v>7555</v>
+      </c>
+      <c r="F30" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="G30" s="36">
+        <v>29188186</v>
+      </c>
+      <c r="H30" t="s">
+        <v>7532</v>
+      </c>
+      <c r="I30" t="s">
+        <v>7532</v>
+      </c>
       <c r="J30" t="b">
         <v>0</v>
       </c>
       <c r="K30" t="b">
         <v>0</v>
       </c>
-      <c r="L30" s="10">
+      <c r="L30" s="41">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1077</v>
+      </c>
+      <c r="M30" s="30" t="s">
+        <v>7600</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="30"/>
-      <c r="D31" s="5"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="36"/>
+      <c r="A31" s="30" t="s">
+        <v>7558</v>
+      </c>
+      <c r="B31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="30" t="s">
+        <v>7610</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E31" s="30" t="s">
+        <v>7561</v>
+      </c>
+      <c r="F31" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="G31" s="39">
+        <v>33294367</v>
+      </c>
+      <c r="H31" t="s">
+        <v>7418</v>
+      </c>
+      <c r="I31" t="s">
+        <v>7532</v>
+      </c>
       <c r="J31" t="b">
         <v>0</v>
       </c>
       <c r="K31" t="b">
         <v>0</v>
       </c>
-      <c r="L31" s="10">
+      <c r="L31" s="41">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1490</v>
+      </c>
+      <c r="M31" t="s">
+        <v>7559</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="30"/>
-      <c r="D32" s="5"/>
-      <c r="F32" s="37"/>
-      <c r="G32" s="36"/>
+      <c r="A32" s="30" t="s">
+        <v>7564</v>
+      </c>
+      <c r="B32" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="30" t="s">
+        <v>7610</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E32" s="30" t="s">
+        <v>7570</v>
+      </c>
+      <c r="F32" s="37" t="s">
+        <v>7469</v>
+      </c>
+      <c r="G32" s="36" t="s">
+        <v>7565</v>
+      </c>
+      <c r="H32" t="s">
+        <v>7566</v>
+      </c>
+      <c r="I32" t="s">
+        <v>7419</v>
+      </c>
       <c r="J32" t="b">
         <v>0</v>
       </c>
       <c r="K32" t="b">
         <v>0</v>
       </c>
-      <c r="L32" s="10">
+      <c r="L32" s="41">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="30"/>
-      <c r="D33" s="5"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="36"/>
+        <v>1709</v>
+      </c>
+      <c r="M32" s="30" t="s">
+        <v>7567</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="30" t="s">
+        <v>7562</v>
+      </c>
+      <c r="B33" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="30" t="s">
+        <v>7610</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E33" s="30" t="s">
+        <v>7571</v>
+      </c>
+      <c r="F33" s="37" t="s">
+        <v>7469</v>
+      </c>
+      <c r="G33" s="36" t="s">
+        <v>7565</v>
+      </c>
+      <c r="H33" t="s">
+        <v>7566</v>
+      </c>
+      <c r="I33" t="s">
+        <v>7419</v>
+      </c>
       <c r="J33" t="b">
         <v>0</v>
       </c>
       <c r="K33" t="b">
         <v>0</v>
       </c>
-      <c r="L33" s="10">
+      <c r="L33" s="41">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="30"/>
-      <c r="D34" s="5"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="36"/>
+        <v>1784</v>
+      </c>
+      <c r="M33" t="s">
+        <v>7568</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="30" t="s">
+        <v>7563</v>
+      </c>
+      <c r="B34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" s="30" t="s">
+        <v>7610</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" s="30" t="s">
+        <v>7572</v>
+      </c>
+      <c r="F34" s="37" t="s">
+        <v>7469</v>
+      </c>
+      <c r="G34" s="36" t="s">
+        <v>7565</v>
+      </c>
+      <c r="H34" t="s">
+        <v>7566</v>
+      </c>
+      <c r="I34" t="s">
+        <v>7419</v>
+      </c>
       <c r="J34" t="b">
         <v>0</v>
       </c>
       <c r="K34" t="b">
         <v>0</v>
       </c>
-      <c r="L34" s="10">
+      <c r="L34" s="41">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="30"/>
-      <c r="D35" s="5"/>
-      <c r="F35" s="37"/>
-      <c r="G35" s="36"/>
+        <v>1223</v>
+      </c>
+      <c r="M34" s="30" t="s">
+        <v>7569</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="30" t="s">
+        <v>7603</v>
+      </c>
+      <c r="B35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="30" t="s">
+        <v>7610</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E35" s="30" t="s">
+        <v>7607</v>
+      </c>
+      <c r="F35" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="G35" s="36">
+        <v>36973546</v>
+      </c>
+      <c r="H35" t="s">
+        <v>7417</v>
+      </c>
+      <c r="I35" t="s">
+        <v>7418</v>
+      </c>
       <c r="J35" t="b">
         <v>0</v>
       </c>
       <c r="K35" t="b">
         <v>0</v>
       </c>
-      <c r="L35" s="10">
+      <c r="L35" s="41">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="30"/>
-      <c r="D36" s="5"/>
-      <c r="F36" s="37"/>
-      <c r="G36" s="36"/>
+        <v>763</v>
+      </c>
+      <c r="M35" t="s">
+        <v>7604</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="30" t="s">
+        <v>7573</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1683</v>
+      </c>
+      <c r="C36" s="30" t="s">
+        <v>7612</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>7460</v>
+      </c>
+      <c r="E36" s="30" t="s">
+        <v>7608</v>
+      </c>
+      <c r="F36" s="37" t="s">
+        <v>7529</v>
+      </c>
+      <c r="G36" s="46" t="s">
+        <v>7602</v>
+      </c>
+      <c r="H36" t="s">
+        <v>7417</v>
+      </c>
+      <c r="I36" t="s">
+        <v>7601</v>
+      </c>
       <c r="J36" t="b">
         <v>0</v>
       </c>
       <c r="K36" t="b">
         <v>0</v>
       </c>
-      <c r="L36" s="10">
+      <c r="L36" s="41">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="30"/>
-      <c r="D37" s="5"/>
-      <c r="F37" s="37"/>
-      <c r="G37" s="36"/>
+        <v>310</v>
+      </c>
+      <c r="M36" t="s">
+        <v>7581</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="30" t="s">
+        <v>7574</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1683</v>
+      </c>
+      <c r="C37" s="30" t="s">
+        <v>7610</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>7460</v>
+      </c>
+      <c r="E37" s="30" t="s">
+        <v>7609</v>
+      </c>
+      <c r="F37" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="G37" s="36">
+        <v>30314480</v>
+      </c>
+      <c r="H37" t="s">
+        <v>7417</v>
+      </c>
+      <c r="I37" t="s">
+        <v>7601</v>
+      </c>
       <c r="J37" t="b">
         <v>0</v>
       </c>
       <c r="K37" t="b">
         <v>0</v>
       </c>
-      <c r="L37" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="30"/>
-      <c r="D38" s="5"/>
-      <c r="G38" s="5"/>
+      <c r="L37" s="41">
+        <f t="shared" ref="L37:L68" si="1">LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M37,CHAR(160)," ")," ",""))))</f>
+        <v>397</v>
+      </c>
+      <c r="M37" t="s">
+        <v>7582</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="30" t="s">
+        <v>7575</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1683</v>
+      </c>
+      <c r="C38" s="30" t="s">
+        <v>7610</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>7460</v>
+      </c>
+      <c r="E38" s="30" t="s">
+        <v>7609</v>
+      </c>
+      <c r="F38" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="G38" s="36">
+        <v>36527112</v>
+      </c>
+      <c r="H38" t="s">
+        <v>7417</v>
+      </c>
+      <c r="I38" t="s">
+        <v>7601</v>
+      </c>
       <c r="J38" t="b">
         <v>0</v>
       </c>
       <c r="K38" t="b">
         <v>0</v>
       </c>
-      <c r="L38" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="30"/>
-      <c r="D39" s="5"/>
-      <c r="G39" s="5"/>
+      <c r="L38" s="41">
+        <f t="shared" si="1"/>
+        <v>406</v>
+      </c>
+      <c r="M38" s="30" t="s">
+        <v>7583</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="30" t="s">
+        <v>7576</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1683</v>
+      </c>
+      <c r="C39" s="30" t="s">
+        <v>7610</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>7460</v>
+      </c>
+      <c r="E39" s="30" t="s">
+        <v>7609</v>
+      </c>
+      <c r="F39" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="G39" s="36">
+        <v>28252957</v>
+      </c>
+      <c r="H39" t="s">
+        <v>7417</v>
+      </c>
+      <c r="I39" t="s">
+        <v>7601</v>
+      </c>
       <c r="J39" t="b">
         <v>0</v>
       </c>
       <c r="K39" t="b">
         <v>0</v>
       </c>
-      <c r="L39" s="10">
+      <c r="L39" s="41">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="30"/>
-      <c r="D40" s="5"/>
-      <c r="G40" s="5"/>
+        <v>310</v>
+      </c>
+      <c r="M39" s="30" t="s">
+        <v>7584</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="30" t="s">
+        <v>7577</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1683</v>
+      </c>
+      <c r="C40" s="30" t="s">
+        <v>7610</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>7460</v>
+      </c>
+      <c r="E40" s="30" t="s">
+        <v>7609</v>
+      </c>
+      <c r="F40" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="G40" s="36">
+        <v>28252958</v>
+      </c>
+      <c r="H40" t="s">
+        <v>7417</v>
+      </c>
+      <c r="I40" t="s">
+        <v>7601</v>
+      </c>
       <c r="J40" t="b">
         <v>0</v>
       </c>
       <c r="K40" t="b">
         <v>0</v>
       </c>
-      <c r="L40" s="10">
-        <f t="shared" si="0"/>
+      <c r="L40" s="41">
+        <f t="shared" si="1"/>
+        <v>310</v>
+      </c>
+      <c r="M40" s="45" t="s">
+        <v>7585</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="30" t="s">
+        <v>7578</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1683</v>
+      </c>
+      <c r="C41" s="30" t="s">
+        <v>7610</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>7460</v>
+      </c>
+      <c r="E41" s="30" t="s">
+        <v>7609</v>
+      </c>
+      <c r="F41" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="G41" s="36">
+        <v>28252959</v>
+      </c>
+      <c r="H41" t="s">
+        <v>7417</v>
+      </c>
+      <c r="I41" t="s">
+        <v>7601</v>
+      </c>
+      <c r="J41" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="K41" t="b">
+        <v>0</v>
+      </c>
+      <c r="L41" s="41">
+        <f t="shared" si="1"/>
+        <v>313</v>
+      </c>
+      <c r="M41" s="45" t="s">
+        <v>7586</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="30" t="s">
+        <v>7579</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1683</v>
+      </c>
+      <c r="C42" s="30" t="s">
+        <v>7610</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>7460</v>
+      </c>
+      <c r="E42" s="30" t="s">
+        <v>7609</v>
+      </c>
+      <c r="F42" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="G42" s="36">
+        <v>28252960</v>
+      </c>
+      <c r="H42" t="s">
+        <v>7417</v>
+      </c>
+      <c r="I42" t="s">
+        <v>7601</v>
+      </c>
+      <c r="J42" t="b">
+        <v>0</v>
+      </c>
+      <c r="K42" t="b">
+        <v>0</v>
+      </c>
+      <c r="L42" s="41">
+        <f t="shared" si="1"/>
+        <v>310</v>
+      </c>
+      <c r="M42" s="45" t="s">
+        <v>7587</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="30" t="s">
+        <v>7580</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1683</v>
+      </c>
+      <c r="C43" s="30" t="s">
+        <v>7610</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>7460</v>
+      </c>
+      <c r="E43" s="30" t="s">
+        <v>7609</v>
+      </c>
+      <c r="F43" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="G43" s="36">
+        <v>28252961</v>
+      </c>
+      <c r="H43" t="s">
+        <v>7417</v>
+      </c>
+      <c r="I43" t="s">
+        <v>7601</v>
+      </c>
+      <c r="J43" t="b">
+        <v>0</v>
+      </c>
+      <c r="K43" t="b">
+        <v>0</v>
+      </c>
+      <c r="L43" s="41">
+        <f t="shared" si="1"/>
+        <v>327</v>
+      </c>
+      <c r="M43" s="45" t="s">
+        <v>7588</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J44" t="b">
+        <v>0</v>
+      </c>
+      <c r="K44" t="b">
+        <v>0</v>
+      </c>
+      <c r="L44" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M44" s="45"/>
+    </row>
+    <row r="45" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J45" t="b">
+        <v>0</v>
+      </c>
+      <c r="K45" t="b">
+        <v>0</v>
+      </c>
+      <c r="L45" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M45" s="45"/>
+    </row>
+    <row r="46" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J46" t="b">
+        <v>0</v>
+      </c>
+      <c r="K46" t="b">
+        <v>0</v>
+      </c>
+      <c r="L46" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M46" s="45"/>
+    </row>
+    <row r="47" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J47" t="b">
+        <v>0</v>
+      </c>
+      <c r="K47" t="b">
+        <v>0</v>
+      </c>
+      <c r="L47" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M47" s="45"/>
+    </row>
+    <row r="48" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J48" t="b">
+        <v>0</v>
+      </c>
+      <c r="K48" t="b">
+        <v>0</v>
+      </c>
+      <c r="L48" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M48" s="45"/>
+    </row>
+    <row r="49" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J49" t="b">
+        <v>0</v>
+      </c>
+      <c r="K49" t="b">
+        <v>0</v>
+      </c>
+      <c r="L49" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M49" s="45"/>
+    </row>
+    <row r="50" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J50" t="b">
+        <v>0</v>
+      </c>
+      <c r="K50" t="b">
+        <v>0</v>
+      </c>
+      <c r="L50" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M50" s="45"/>
+    </row>
+    <row r="51" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J51" t="b">
+        <v>0</v>
+      </c>
+      <c r="K51" t="b">
+        <v>0</v>
+      </c>
+      <c r="L51" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M51" s="45"/>
+    </row>
+    <row r="52" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J52" t="b">
+        <v>0</v>
+      </c>
+      <c r="K52" t="b">
+        <v>0</v>
+      </c>
+      <c r="L52" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M52" s="45"/>
+    </row>
+    <row r="53" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J53" t="b">
+        <v>0</v>
+      </c>
+      <c r="K53" t="b">
+        <v>0</v>
+      </c>
+      <c r="L53" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M53" s="45"/>
+    </row>
+    <row r="54" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K54" t="b">
+        <v>0</v>
+      </c>
+      <c r="L54" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M54" s="45"/>
+    </row>
+    <row r="55" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J55" t="b">
+        <v>0</v>
+      </c>
+      <c r="K55" t="b">
+        <v>0</v>
+      </c>
+      <c r="L55" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M55" s="45"/>
+    </row>
+    <row r="56" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J56" t="b">
+        <v>0</v>
+      </c>
+      <c r="K56" t="b">
+        <v>0</v>
+      </c>
+      <c r="L56" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M56" s="45"/>
+    </row>
+    <row r="57" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J57" t="b">
+        <v>0</v>
+      </c>
+      <c r="K57" t="b">
+        <v>0</v>
+      </c>
+      <c r="L57" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M57" s="45"/>
+    </row>
+    <row r="58" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J58" t="b">
+        <v>0</v>
+      </c>
+      <c r="K58" t="b">
+        <v>0</v>
+      </c>
+      <c r="L58" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M58" s="45"/>
+    </row>
+    <row r="59" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="30"/>
+      <c r="D59" s="5"/>
+      <c r="F59" s="37"/>
+      <c r="G59" s="36"/>
+      <c r="J59" t="b">
+        <v>0</v>
+      </c>
+      <c r="K59" t="b">
+        <v>0</v>
+      </c>
+      <c r="L59" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="30"/>
+      <c r="D60" s="5"/>
+      <c r="F60" s="37"/>
+      <c r="G60" s="36"/>
+      <c r="J60" t="b">
+        <v>0</v>
+      </c>
+      <c r="K60" t="b">
+        <v>0</v>
+      </c>
+      <c r="L60" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="30"/>
+      <c r="D61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="J61" t="b">
+        <v>0</v>
+      </c>
+      <c r="K61" t="b">
+        <v>0</v>
+      </c>
+      <c r="L61" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="30"/>
+      <c r="D62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="J62" t="b">
+        <v>0</v>
+      </c>
+      <c r="K62" t="b">
+        <v>0</v>
+      </c>
+      <c r="L62" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="30"/>
+      <c r="D63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="J63" t="b">
+        <v>0</v>
+      </c>
+      <c r="K63" t="b">
+        <v>0</v>
+      </c>
+      <c r="L63" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="30"/>
+      <c r="D64" s="5"/>
+      <c r="F64" s="37"/>
+      <c r="G64" s="36"/>
+      <c r="J64" t="b">
+        <v>0</v>
+      </c>
+      <c r="K64" t="b">
+        <v>0</v>
+      </c>
+      <c r="L64" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="30"/>
+      <c r="D65" s="5"/>
+      <c r="F65" s="37"/>
+      <c r="G65" s="36"/>
+      <c r="J65" t="b">
+        <v>0</v>
+      </c>
+      <c r="K65" t="b">
+        <v>0</v>
+      </c>
+      <c r="L65" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="30"/>
+      <c r="D66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="J66" t="b">
+        <v>0</v>
+      </c>
+      <c r="K66" t="b">
+        <v>0</v>
+      </c>
+      <c r="L66" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="30"/>
+      <c r="D67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="J67" t="b">
+        <v>0</v>
+      </c>
+      <c r="K67" t="b">
+        <v>0</v>
+      </c>
+      <c r="L67" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="30"/>
+      <c r="D68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="J68" t="b">
+        <v>0</v>
+      </c>
+      <c r="K68" t="b">
+        <v>0</v>
+      </c>
+      <c r="L68" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -25403,43 +26529,46 @@
   <mergeCells count="1">
     <mergeCell ref="A5:F5"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G36" r:id="rId1" xr:uid="{B5CDEE4F-FBA5-CD48-B4D6-0AF10CCFA772}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
+          <x14:formula1>
+            <xm:f>'Ontology Terms'!$F$2:$F$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>J15:K68</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
             <xm:f>Sequence_alteration_terms!$A$2:$A$19</xm:f>
           </x14:formula1>
-          <xm:sqref>D15:D40</xm:sqref>
+          <xm:sqref>D15:D43 D59:D68</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
+          <x14:formula1>
+            <xm:f>'Ontology Terms'!$B$2:$B$2518</xm:f>
+          </x14:formula1>
+          <xm:sqref>B15:B43 B59:B68</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
+          <x14:formula1>
+            <xm:f>'Organism Terms'!$A$2:$A$34</xm:f>
+          </x14:formula1>
+          <xm:sqref>H59:I68 H15:I43</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>data_source!$B$2:$B$11</xm:f>
           </x14:formula1>
-          <xm:sqref>F15:F40</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
-          <x14:formula1>
-            <xm:f>'Organism Terms'!$A$2:$A$34</xm:f>
-          </x14:formula1>
-          <xm:sqref>H15:I40</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
-          <x14:formula1>
-            <xm:f>'Ontology Terms'!$B$2:$B$2518</xm:f>
-          </x14:formula1>
-          <xm:sqref>B15:B40</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
-          <x14:formula1>
-            <xm:f>'Ontology Terms'!$F$2:$F$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>J15:K40</xm:sqref>
+          <xm:sqref>F59:F68 F15:F43</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -25831,8 +26960,8 @@
   </sheetPr>
   <dimension ref="A1:F2535"/>
   <sheetViews>
-    <sheetView topLeftCell="A1355" workbookViewId="0">
-      <selection activeCell="C1638" sqref="C1638"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -60510,7 +61639,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A30" sqref="A30"/>
+      <selection pane="bottomRight" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -60760,7 +61889,16 @@
         <v>7532</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>7566</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>7601</v>
+      </c>
+    </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Minor correction to file name
</commit_message>
<xml_diff>
--- a/Open-Yeast-Collection-IIA-new-parts.xlsx
+++ b/Open-Yeast-Collection-IIA-new-parts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rover/Sync/GitHub/Open-Yeast-Collection-IIA-new-parts-package/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D85C40F-3BBA-4E41-8FE4-2A96EE87D992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70023167-DFD1-A445-B4A2-DECD620D5B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="26660" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="500" windowWidth="26660" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -22746,12 +22746,6 @@
     <t>ggcGAAGACagGGAGcTTAATTAAcTCTAGAcAGACtGAGACCctcgagggagTTGACGGCTAGCTCAGTCCTAGGTACAGTGCTAGCgtacTTGTTTAACTTTAAGAAGGAGatatacaATGGTAGCCCGTAAAGGCGAgGAGCTGTTCACTGGTGTCGTCCCTATTCTGGTGGAACTGGATGGTGATGTCAACGGTCATAAGTTTTCCGTGCGTGGCGAGGGTGAAGGTGACGCAACTAATGGTAAACTGACGCTGAAGTTCATCTGTACTACTGGTAAACTGCCGGTACCTTGGCCGACTCTGGTAACGACGCTGACTTATGGTGTTCAGTGCTTTGCTCGTTATCCGGACCATATGAAGCAGCATGACTTCTTCAAGTCCGCCATGCCGGAAGGCTATGTGCAGGAACGCACGATTTCCTTTAAGGATGACGGCACGTACAAAACGCGTGCGGAAGTGAAATTTGAAGGCGATACCCTGGTAAACCGCATTGAGCTGAAAGGCATTGACTTTAAAGAAGATGGCAATATCCTGGGCCATAAGCTGGAATACAATTTTAACAGCCACAATGTTTACATCACCGCCGATAAACAAAAAAATGGCATTAAAGCGAATTTTAAAATTCGCCACAACGTGGAGGATGGCAGCGTGCAGCTGGCTGATCACTACCAGCAAAACACTCCAATCGGTGATGGTCCTGTTCTGCTGCCAGACAATCACTATCTGAGCACGCAAAGCGTTCTGTCTAAAGATCCGAACGAGAAACGCGATCATATGGTTCTGCTGGAGTTCGTAACCGCAGCGGGCATCACGCATGGTATGGATGAACTGTACAAAGGTTCGTAActtctgactgagttgcacgctcaattgGGTCTCtATGAactagtcgCGCTtcGTCTTCtga</t>
   </si>
   <si>
-    <t>yl_pTEF_274-part</t>
-  </si>
-  <si>
-    <t>yl_UAS1B-part</t>
-  </si>
-  <si>
     <t>Yarrowia lipolytica promoter for GGA with the Open Yeast Collection</t>
   </si>
   <si>
@@ -22854,24 +22848,6 @@
     <t>ggcGAAGACagGGAGcTTAATTAAcTCTAGAcGGTCTCcTACTatgaccaaaccaacgcaagtcttagttcgttcagtctctattttattcttcatcacactgttgcacttggttgttgcaatgagatttcctagtattttcactgctgtgctatttgccgctagttccgctctagctgctccagttaatactactactgaagatgaattggagggtgacttcgatgttgctgttctgcctttttccgcttctatcgcagccaaggaagaaggtgtatccctagagaagcgttCCATgGAGACCactagtcgCGCTtcGTCTTCtga</t>
   </si>
   <si>
-    <t>yl_pACL2-part</t>
-  </si>
-  <si>
-    <t>yl_pDGA1-part</t>
-  </si>
-  <si>
-    <t>yl_pGAPDH-part</t>
-  </si>
-  <si>
-    <t>yl_pICL-part</t>
-  </si>
-  <si>
-    <t>yl_pIDH2-part</t>
-  </si>
-  <si>
-    <t>yl_pLIP2-part</t>
-  </si>
-  <si>
     <t>ggcGAAGACagGGAGcTTAATTAAcTCTAGAcGGTCTCtGGAGaaaatgacgacaattcgaaccgaggccaattgagcacgccgaagcagtttcaacgcaatcggccgcgattcggaccagttgggccgctcttaggcagtcaccaaccagatgttctgcacggatttccccgattgtggaaatgaaatcgacgccggcgtcatggcaatcgacagttgggggagagataaatcggtggtcacgtgtacaccccccacgagcgActcccgtgccactttctccccagcgaccgttatctcaactcacttcccctctctcaacagttaacccaaccctcaaccaaattgacgtggttagcggtttggcaggcgacaagcgaaattgacttttccaacaaactcagcacgccaccacgcccgttcgccatgcatgttgtacccctcaccgaggccaccaggattgggtcaaagtgagggggagtatcaacaagaaggaaaaagggtcttttgggagctccaaaatagttggggaggcggaccaacagagacatatatagactcgaaaccaatgtcacaaatccatctttaccaaataaagttagggacacaaaaccgctctccaaacaggatataattgtcccaccaccaccacacacacacaccacccaacccaacatttagcctccgtctgctacaacttaatcaggcacgactcactcttctttctacgtgacacaaacagagcgacacctacggagcgacacccccctcgaccgacacagaaacagcgtcgatcacacacacacacacacacacaccgaatccgacactcaccagatcaatcTACTtGAGACCactagtcgCGCTtcGTCTTCtga</t>
   </si>
   <si>
@@ -22954,6 +22930,30 @@
   </si>
   <si>
     <t>total bp</t>
+  </si>
+  <si>
+    <t>AB_yl_pACL2-part</t>
+  </si>
+  <si>
+    <t>AB_yl_pDGA1-part</t>
+  </si>
+  <si>
+    <t>AB_yl_pGAPDH-part</t>
+  </si>
+  <si>
+    <t>AB_yl_pICL-part</t>
+  </si>
+  <si>
+    <t>AB_yl_pIDH2-part</t>
+  </si>
+  <si>
+    <t>AB_yl_pLIP2-part</t>
+  </si>
+  <si>
+    <t>A2B_yl_pTEF_274-part</t>
+  </si>
+  <si>
+    <t>AA2_yl_UAS1B-part</t>
   </si>
 </sst>
 </file>
@@ -23282,7 +23282,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -23339,12 +23339,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -23354,6 +23348,11 @@
     <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -23811,10 +23810,10 @@
   <dimension ref="A1:M963"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="14" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="14" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="M11" sqref="M11"/>
+      <selection pane="bottomRight" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -23874,12 +23873,12 @@
       <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:13" ht="46" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="42"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="44"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="47"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -23974,8 +23973,8 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L10" s="48" t="s">
-        <v>7616</v>
+      <c r="L10" s="44" t="s">
+        <v>7608</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -23986,7 +23985,7 @@
         <f>SUM(L15:L59)</f>
         <v>19953</v>
       </c>
-      <c r="M11" s="47">
+      <c r="M11" s="43">
         <f>20000-L11</f>
         <v>47</v>
       </c>
@@ -24084,13 +24083,13 @@
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="30" t="s">
-        <v>7607</v>
+        <v>7599</v>
       </c>
       <c r="B15" s="30" t="s">
         <v>52</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>7604</v>
+        <v>7596</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>7445</v>
@@ -24126,13 +24125,13 @@
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="30" t="s">
-        <v>7608</v>
+        <v>7600</v>
       </c>
       <c r="B16" s="30" t="s">
         <v>52</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>7604</v>
+        <v>7596</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>7445</v>
@@ -24168,13 +24167,13 @@
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="30" t="s">
-        <v>7609</v>
+        <v>7601</v>
       </c>
       <c r="B17" s="30" t="s">
         <v>52</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>7604</v>
+        <v>7596</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>7445</v>
@@ -24210,13 +24209,13 @@
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="30" t="s">
-        <v>7610</v>
+        <v>7602</v>
       </c>
       <c r="B18" s="30" t="s">
         <v>52</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>7604</v>
+        <v>7596</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>7445</v>
@@ -24252,13 +24251,13 @@
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="30" t="s">
-        <v>7611</v>
+        <v>7603</v>
       </c>
       <c r="B19" s="30" t="s">
         <v>52</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>7604</v>
+        <v>7596</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>7445</v>
@@ -24294,13 +24293,13 @@
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="30" t="s">
-        <v>7612</v>
+        <v>7604</v>
       </c>
       <c r="B20" s="30" t="s">
         <v>52</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>7604</v>
+        <v>7596</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>7445</v>
@@ -24342,13 +24341,13 @@
         <v>1683</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>7604</v>
+        <v>7596</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>7460</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>7600</v>
+        <v>7592</v>
       </c>
       <c r="F21" s="37" t="s">
         <v>7485</v>
@@ -24384,13 +24383,13 @@
         <v>1683</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>7604</v>
+        <v>7596</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>7460</v>
       </c>
       <c r="E22" s="30" t="s">
-        <v>7599</v>
+        <v>7591</v>
       </c>
       <c r="F22" s="37" t="s">
         <v>7485</v>
@@ -24420,19 +24419,19 @@
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="30" t="s">
-        <v>7547</v>
+        <v>7615</v>
       </c>
       <c r="B23" t="s">
         <v>41</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>7604</v>
+        <v>7596</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>7445</v>
       </c>
       <c r="E23" s="30" t="s">
-        <v>7549</v>
+        <v>7547</v>
       </c>
       <c r="F23" s="37" t="s">
         <v>39</v>
@@ -24457,24 +24456,24 @@
         <v>351</v>
       </c>
       <c r="M23" t="s">
-        <v>7554</v>
+        <v>7552</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="30" t="s">
-        <v>7548</v>
+        <v>7616</v>
       </c>
       <c r="B24" t="s">
         <v>1728</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>7605</v>
+        <v>7597</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>7460</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>7550</v>
+        <v>7548</v>
       </c>
       <c r="F24" s="37" t="s">
         <v>39</v>
@@ -24499,24 +24498,24 @@
         <v>310</v>
       </c>
       <c r="M24" t="s">
-        <v>7551</v>
+        <v>7549</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="30" t="s">
-        <v>7583</v>
+        <v>7609</v>
       </c>
       <c r="B25" t="s">
         <v>41</v>
       </c>
       <c r="C25" s="30" t="s">
-        <v>7604</v>
+        <v>7596</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>7445</v>
       </c>
       <c r="E25" t="s">
-        <v>7549</v>
+        <v>7547</v>
       </c>
       <c r="F25" s="37" t="s">
         <v>39</v>
@@ -24541,24 +24540,24 @@
         <v>878</v>
       </c>
       <c r="M25" s="30" t="s">
-        <v>7589</v>
+        <v>7581</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="30" t="s">
-        <v>7584</v>
+        <v>7610</v>
       </c>
       <c r="B26" t="s">
         <v>41</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>7604</v>
+        <v>7596</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>7445</v>
       </c>
       <c r="E26" t="s">
-        <v>7549</v>
+        <v>7547</v>
       </c>
       <c r="F26" s="37" t="s">
         <v>39</v>
@@ -24583,24 +24582,24 @@
         <v>877</v>
       </c>
       <c r="M26" s="30" t="s">
-        <v>7590</v>
+        <v>7582</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="30" t="s">
-        <v>7585</v>
+        <v>7611</v>
       </c>
       <c r="B27" t="s">
         <v>41</v>
       </c>
       <c r="C27" s="30" t="s">
-        <v>7604</v>
+        <v>7596</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>7445</v>
       </c>
       <c r="E27" t="s">
-        <v>7549</v>
+        <v>7547</v>
       </c>
       <c r="F27" s="37" t="s">
         <v>39</v>
@@ -24625,24 +24624,24 @@
         <v>880</v>
       </c>
       <c r="M27" s="30" t="s">
-        <v>7591</v>
+        <v>7583</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="30" t="s">
-        <v>7586</v>
+        <v>7612</v>
       </c>
       <c r="B28" t="s">
         <v>41</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>7604</v>
+        <v>7596</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>7445</v>
       </c>
       <c r="E28" t="s">
-        <v>7549</v>
+        <v>7547</v>
       </c>
       <c r="F28" s="37" t="s">
         <v>39</v>
@@ -24667,24 +24666,24 @@
         <v>1085</v>
       </c>
       <c r="M28" s="30" t="s">
-        <v>7592</v>
+        <v>7584</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="30" t="s">
-        <v>7587</v>
+        <v>7613</v>
       </c>
       <c r="B29" t="s">
         <v>41</v>
       </c>
       <c r="C29" s="30" t="s">
-        <v>7604</v>
+        <v>7596</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>7445</v>
       </c>
       <c r="E29" t="s">
-        <v>7549</v>
+        <v>7547</v>
       </c>
       <c r="F29" s="37" t="s">
         <v>39</v>
@@ -24709,24 +24708,24 @@
         <v>877</v>
       </c>
       <c r="M29" s="30" t="s">
-        <v>7593</v>
+        <v>7585</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="30" t="s">
-        <v>7588</v>
+        <v>7614</v>
       </c>
       <c r="B30" t="s">
         <v>41</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>7604</v>
+        <v>7596</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>7445</v>
       </c>
       <c r="E30" t="s">
-        <v>7549</v>
+        <v>7547</v>
       </c>
       <c r="F30" s="37" t="s">
         <v>39</v>
@@ -24751,24 +24750,24 @@
         <v>1077</v>
       </c>
       <c r="M30" s="30" t="s">
-        <v>7594</v>
+        <v>7586</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="30" t="s">
-        <v>7552</v>
+        <v>7550</v>
       </c>
       <c r="B31" t="s">
         <v>47</v>
       </c>
       <c r="C31" s="30" t="s">
-        <v>7604</v>
+        <v>7596</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>48</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>7555</v>
+        <v>7553</v>
       </c>
       <c r="F31" s="37" t="s">
         <v>39</v>
@@ -24793,33 +24792,33 @@
         <v>1490</v>
       </c>
       <c r="M31" t="s">
-        <v>7553</v>
+        <v>7551</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="30" t="s">
-        <v>7558</v>
+        <v>7556</v>
       </c>
       <c r="B32" t="s">
         <v>47</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>7604</v>
+        <v>7596</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>48</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>7564</v>
+        <v>7562</v>
       </c>
       <c r="F32" s="37" t="s">
         <v>7469</v>
       </c>
       <c r="G32" s="36" t="s">
-        <v>7559</v>
+        <v>7557</v>
       </c>
       <c r="H32" t="s">
-        <v>7560</v>
+        <v>7558</v>
       </c>
       <c r="I32" t="s">
         <v>7419</v>
@@ -24835,33 +24834,33 @@
         <v>1709</v>
       </c>
       <c r="M32" s="30" t="s">
-        <v>7561</v>
+        <v>7559</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="30" t="s">
-        <v>7556</v>
+        <v>7554</v>
       </c>
       <c r="B33" t="s">
         <v>47</v>
       </c>
       <c r="C33" s="30" t="s">
-        <v>7604</v>
+        <v>7596</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>48</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>7565</v>
+        <v>7563</v>
       </c>
       <c r="F33" s="37" t="s">
         <v>7469</v>
       </c>
       <c r="G33" s="36" t="s">
-        <v>7559</v>
+        <v>7557</v>
       </c>
       <c r="H33" t="s">
-        <v>7560</v>
+        <v>7558</v>
       </c>
       <c r="I33" t="s">
         <v>7419</v>
@@ -24877,33 +24876,33 @@
         <v>1784</v>
       </c>
       <c r="M33" t="s">
-        <v>7562</v>
+        <v>7560</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="30" t="s">
-        <v>7557</v>
+        <v>7555</v>
       </c>
       <c r="B34" t="s">
         <v>47</v>
       </c>
       <c r="C34" s="30" t="s">
-        <v>7604</v>
+        <v>7596</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>48</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>7566</v>
+        <v>7564</v>
       </c>
       <c r="F34" s="37" t="s">
         <v>7469</v>
       </c>
       <c r="G34" s="36" t="s">
-        <v>7559</v>
+        <v>7557</v>
       </c>
       <c r="H34" t="s">
-        <v>7560</v>
+        <v>7558</v>
       </c>
       <c r="I34" t="s">
         <v>7419</v>
@@ -24919,24 +24918,24 @@
         <v>1223</v>
       </c>
       <c r="M34" s="30" t="s">
-        <v>7563</v>
+        <v>7561</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="30" t="s">
-        <v>7597</v>
+        <v>7589</v>
       </c>
       <c r="B35" t="s">
         <v>47</v>
       </c>
       <c r="C35" s="30" t="s">
-        <v>7604</v>
+        <v>7596</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>48</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>7601</v>
+        <v>7593</v>
       </c>
       <c r="F35" s="37" t="s">
         <v>39</v>
@@ -24961,36 +24960,36 @@
         <v>763</v>
       </c>
       <c r="M35" t="s">
-        <v>7598</v>
+        <v>7590</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="30" t="s">
-        <v>7567</v>
+        <v>7565</v>
       </c>
       <c r="B36" t="s">
         <v>1683</v>
       </c>
       <c r="C36" s="30" t="s">
-        <v>7606</v>
+        <v>7598</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>7460</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>7602</v>
+        <v>7594</v>
       </c>
       <c r="F36" s="37" t="s">
         <v>7529</v>
       </c>
-      <c r="G36" s="46" t="s">
-        <v>7596</v>
+      <c r="G36" s="42" t="s">
+        <v>7588</v>
       </c>
       <c r="H36" t="s">
         <v>7417</v>
       </c>
       <c r="I36" t="s">
-        <v>7595</v>
+        <v>7587</v>
       </c>
       <c r="J36" t="b">
         <v>0</v>
@@ -25003,24 +25002,24 @@
         <v>310</v>
       </c>
       <c r="M36" t="s">
-        <v>7575</v>
+        <v>7573</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="30" t="s">
-        <v>7568</v>
+        <v>7566</v>
       </c>
       <c r="B37" t="s">
         <v>1683</v>
       </c>
       <c r="C37" s="30" t="s">
-        <v>7604</v>
+        <v>7596</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>7460</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>7603</v>
+        <v>7595</v>
       </c>
       <c r="F37" s="37" t="s">
         <v>39</v>
@@ -25032,7 +25031,7 @@
         <v>7417</v>
       </c>
       <c r="I37" t="s">
-        <v>7595</v>
+        <v>7587</v>
       </c>
       <c r="J37" t="b">
         <v>0</v>
@@ -25045,24 +25044,24 @@
         <v>397</v>
       </c>
       <c r="M37" t="s">
-        <v>7576</v>
+        <v>7574</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="30" t="s">
-        <v>7569</v>
+        <v>7567</v>
       </c>
       <c r="B38" t="s">
         <v>1683</v>
       </c>
       <c r="C38" s="30" t="s">
-        <v>7604</v>
+        <v>7596</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>7460</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>7603</v>
+        <v>7595</v>
       </c>
       <c r="F38" s="37" t="s">
         <v>39</v>
@@ -25074,7 +25073,7 @@
         <v>7417</v>
       </c>
       <c r="I38" t="s">
-        <v>7595</v>
+        <v>7587</v>
       </c>
       <c r="J38" t="b">
         <v>0</v>
@@ -25087,24 +25086,24 @@
         <v>406</v>
       </c>
       <c r="M38" s="30" t="s">
-        <v>7577</v>
+        <v>7575</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="30" t="s">
-        <v>7570</v>
+        <v>7568</v>
       </c>
       <c r="B39" t="s">
         <v>1683</v>
       </c>
       <c r="C39" s="30" t="s">
-        <v>7604</v>
+        <v>7596</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>7460</v>
       </c>
       <c r="E39" s="30" t="s">
-        <v>7603</v>
+        <v>7595</v>
       </c>
       <c r="F39" s="37" t="s">
         <v>39</v>
@@ -25116,7 +25115,7 @@
         <v>7417</v>
       </c>
       <c r="I39" t="s">
-        <v>7595</v>
+        <v>7587</v>
       </c>
       <c r="J39" t="b">
         <v>0</v>
@@ -25129,24 +25128,24 @@
         <v>310</v>
       </c>
       <c r="M39" s="30" t="s">
-        <v>7578</v>
+        <v>7576</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="30" t="s">
-        <v>7571</v>
+        <v>7569</v>
       </c>
       <c r="B40" t="s">
         <v>1683</v>
       </c>
       <c r="C40" s="30" t="s">
-        <v>7604</v>
+        <v>7596</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>7460</v>
       </c>
       <c r="E40" s="30" t="s">
-        <v>7603</v>
+        <v>7595</v>
       </c>
       <c r="F40" s="37" t="s">
         <v>39</v>
@@ -25158,7 +25157,7 @@
         <v>7417</v>
       </c>
       <c r="I40" t="s">
-        <v>7595</v>
+        <v>7587</v>
       </c>
       <c r="J40" t="b">
         <v>0</v>
@@ -25170,25 +25169,25 @@
         <f t="shared" si="1"/>
         <v>310</v>
       </c>
-      <c r="M40" s="45" t="s">
-        <v>7579</v>
+      <c r="M40" s="30" t="s">
+        <v>7577</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="30" t="s">
-        <v>7572</v>
+        <v>7570</v>
       </c>
       <c r="B41" t="s">
         <v>1683</v>
       </c>
       <c r="C41" s="30" t="s">
-        <v>7604</v>
+        <v>7596</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>7460</v>
       </c>
       <c r="E41" s="30" t="s">
-        <v>7603</v>
+        <v>7595</v>
       </c>
       <c r="F41" s="37" t="s">
         <v>39</v>
@@ -25200,7 +25199,7 @@
         <v>7417</v>
       </c>
       <c r="I41" t="s">
-        <v>7595</v>
+        <v>7587</v>
       </c>
       <c r="J41" t="b">
         <v>0</v>
@@ -25212,25 +25211,25 @@
         <f t="shared" si="1"/>
         <v>313</v>
       </c>
-      <c r="M41" s="45" t="s">
-        <v>7580</v>
+      <c r="M41" s="30" t="s">
+        <v>7578</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="30" t="s">
-        <v>7573</v>
+        <v>7571</v>
       </c>
       <c r="B42" t="s">
         <v>1683</v>
       </c>
       <c r="C42" s="30" t="s">
-        <v>7604</v>
+        <v>7596</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>7460</v>
       </c>
       <c r="E42" s="30" t="s">
-        <v>7603</v>
+        <v>7595</v>
       </c>
       <c r="F42" s="37" t="s">
         <v>39</v>
@@ -25242,7 +25241,7 @@
         <v>7417</v>
       </c>
       <c r="I42" t="s">
-        <v>7595</v>
+        <v>7587</v>
       </c>
       <c r="J42" t="b">
         <v>0</v>
@@ -25254,25 +25253,25 @@
         <f t="shared" si="1"/>
         <v>310</v>
       </c>
-      <c r="M42" s="45" t="s">
-        <v>7581</v>
+      <c r="M42" s="30" t="s">
+        <v>7579</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="30" t="s">
-        <v>7574</v>
+        <v>7572</v>
       </c>
       <c r="B43" t="s">
         <v>1683</v>
       </c>
       <c r="C43" s="30" t="s">
-        <v>7604</v>
+        <v>7596</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>7460</v>
       </c>
       <c r="E43" s="30" t="s">
-        <v>7603</v>
+        <v>7595</v>
       </c>
       <c r="F43" s="37" t="s">
         <v>39</v>
@@ -25284,7 +25283,7 @@
         <v>7417</v>
       </c>
       <c r="I43" t="s">
-        <v>7595</v>
+        <v>7587</v>
       </c>
       <c r="J43" t="b">
         <v>0</v>
@@ -25296,25 +25295,25 @@
         <f t="shared" si="1"/>
         <v>327</v>
       </c>
-      <c r="M43" s="45" t="s">
-        <v>7582</v>
+      <c r="M43" s="30" t="s">
+        <v>7580</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>7613</v>
+        <v>7605</v>
       </c>
       <c r="B44" t="s">
         <v>1683</v>
       </c>
       <c r="C44" s="30" t="s">
-        <v>7604</v>
+        <v>7596</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>7460</v>
       </c>
       <c r="E44" s="30" t="s">
-        <v>7614</v>
+        <v>7606</v>
       </c>
       <c r="F44" s="37" t="s">
         <v>39</v>
@@ -25338,8 +25337,8 @@
         <f t="shared" si="1"/>
         <v>310</v>
       </c>
-      <c r="M44" s="45" t="s">
-        <v>7615</v>
+      <c r="M44" s="30" t="s">
+        <v>7607</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25353,7 +25352,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M45" s="45"/>
+      <c r="M45" s="30"/>
     </row>
     <row r="46" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J46" t="b">
@@ -25366,7 +25365,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M46" s="45"/>
+      <c r="M46" s="30"/>
     </row>
     <row r="47" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J47" t="b">
@@ -25379,7 +25378,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M47" s="45"/>
+      <c r="M47" s="30"/>
     </row>
     <row r="48" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J48" t="b">
@@ -25392,7 +25391,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M48" s="45"/>
+      <c r="M48" s="30"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J49" t="b">
@@ -25405,7 +25404,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M49" s="45"/>
+      <c r="M49" s="30"/>
     </row>
     <row r="50" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J50" t="b">
@@ -25418,7 +25417,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M50" s="45"/>
+      <c r="M50" s="30"/>
     </row>
     <row r="51" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J51" t="b">
@@ -25431,7 +25430,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M51" s="45"/>
+      <c r="M51" s="30"/>
     </row>
     <row r="52" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J52" t="b">
@@ -25444,7 +25443,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M52" s="45"/>
+      <c r="M52" s="30"/>
     </row>
     <row r="53" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J53" t="b">
@@ -25457,7 +25456,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M53" s="45"/>
+      <c r="M53" s="30"/>
     </row>
     <row r="54" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J54" t="b">
@@ -25470,7 +25469,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M54" s="45"/>
+      <c r="M54" s="30"/>
     </row>
     <row r="55" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J55" t="b">
@@ -25483,7 +25482,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M55" s="45"/>
+      <c r="M55" s="30"/>
     </row>
     <row r="56" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J56" t="b">
@@ -25496,7 +25495,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M56" s="45"/>
+      <c r="M56" s="30"/>
     </row>
     <row r="57" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J57" t="b">
@@ -25509,7 +25508,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M57" s="45"/>
+      <c r="M57" s="30"/>
     </row>
     <row r="58" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J58" t="b">
@@ -25522,7 +25521,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M58" s="45"/>
+      <c r="M58" s="30"/>
     </row>
     <row r="59" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="30"/>
@@ -61939,12 +61938,12 @@
     </row>
     <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>7560</v>
+        <v>7558</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>7595</v>
+        <v>7587</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Replaced a terminator part with a BT1 signal peptide.
</commit_message>
<xml_diff>
--- a/Open-Yeast-Collection-IIA-new-parts.xlsx
+++ b/Open-Yeast-Collection-IIA-new-parts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rover/Sync/GitHub/Open-Yeast-Collection-IIA-new-parts-package/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70023167-DFD1-A445-B4A2-DECD620D5B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B4E538-E165-0846-9420-A2536F04C442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="500" windowWidth="26660" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1240" yWindow="500" windowWidth="26660" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7843" uniqueCount="7617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7843" uniqueCount="7618">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22716,9 +22716,6 @@
     <t>ggcGAAGACagGGAGcTTAATTAAcTCTAGAcGGTCTCtGCTTtttgaaagatgatactctttatttctagacagttatataCGCTtGAGACCactagtcgCGCTtcGTCTTCtgatccctgctacagctctgatctgacgctcaactcgtgttcacaaccttggacgatctgacagcatccgcgcacttatctagcaagtttgagaacttcccgctctaagtgcctacggaacttctccgcgttcgatctgcgttgagagtcaacgagagtacggtcctgctacatacctccctatatgagtaacatgt</t>
   </si>
   <si>
-    <t>ggcGAAGACagGGAGcTTAATTAAcTCTAGAcGGTCTCtGCTTgctgcttgtacctagtgcaaccccagtttgttaaaaattagtagtcaaaaacttctgagttaaaaaaaaaaaaaaaaCGCTtGAGACCactagtcgCGCTtcGTCTTCtgactactcttattgccgccttagactacacaacctatcgcacccttagactacgtggtgccgatgtgcaaggttccagaagtcgcctcggatgatctgcattgagagctagaagcgaattatggatccaccacaatggcaaatcaacgtgcctctgtg</t>
-  </si>
-  <si>
     <t>ggcGAAGACagGGAGcTTAATTAAcTCTAGAcGGTCTCtGCTTatcggcccgggcaaaccacaccaacccttctcttctatcgccagtcgaaatgtgactttttaagtaatcaattcttgtaaacacttgatcgtacgtagttggatcatggcgcgacaaaataatttccaaccagtgtcactcactccactcagactgttggagcacttgacagatagatcacccatcaagcagcaacttggaatCGCTtGAGACCactagtcgCGCTtcGTCTTCtgactatagtgtaacgcaggttcgtctgcccta</t>
   </si>
   <si>
@@ -22914,9 +22911,6 @@
     <t>EF_yl_tSynthGuo-part</t>
   </si>
   <si>
-    <t>EF_yl_tTEF-part</t>
-  </si>
-  <si>
     <t>EF_yl_tXPR2-part</t>
   </si>
   <si>
@@ -22954,6 +22948,15 @@
   </si>
   <si>
     <t>AA2_yl_UAS1B-part</t>
+  </si>
+  <si>
+    <t>BT1_Wci_α_mating_factor_signal</t>
+  </si>
+  <si>
+    <t>α-mating factor secretion signal from Wickerhamomyces ciferrii as a BT1 ( TACT/CCAT) part.</t>
+  </si>
+  <si>
+    <t>ggcGAAGACagGGAGcTTAATTAAcTCTAGAcGGTCTCcTACTatgcaactttctttactaacttctttggccattgtttccactttactaggctcttcgtttgctgctccagtggagaatatcaatatcaaagacaatggcaatggcaccagtgaagctgatgttcctggaacttctcaaggtgttgagtttccgtttgccaaagaagccatcattgaagctgtttctttaggcaatgatattgctccaattgttctcaatgatgctgtttattttgtcaataccaccactgttgacaaagagctggaaagcaaacttggcaaacgatCCATgGAGACCactagtcgCGCTtcGTCTTCtga</t>
   </si>
 </sst>
 </file>
@@ -23810,10 +23813,10 @@
   <dimension ref="A1:M963"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="14" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="14" topLeftCell="D18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="A26" sqref="A26"/>
+      <selection pane="bottomRight" activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -23974,7 +23977,7 @@
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L10" s="44" t="s">
-        <v>7608</v>
+        <v>7606</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -23983,11 +23986,11 @@
       </c>
       <c r="L11" s="40">
         <f>SUM(L15:L59)</f>
-        <v>19953</v>
+        <v>20006</v>
       </c>
       <c r="M11" s="43">
         <f>20000-L11</f>
-        <v>47</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -24083,19 +24086,19 @@
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="30" t="s">
-        <v>7599</v>
+        <v>7598</v>
       </c>
       <c r="B15" s="30" t="s">
         <v>52</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>7596</v>
+        <v>7595</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>7445</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>7540</v>
+        <v>7539</v>
       </c>
       <c r="F15" s="37" t="s">
         <v>39</v>
@@ -24120,24 +24123,24 @@
         <v>310</v>
       </c>
       <c r="M15" t="s">
-        <v>7539</v>
+        <v>7538</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="30" t="s">
-        <v>7600</v>
+        <v>7599</v>
       </c>
       <c r="B16" s="30" t="s">
         <v>52</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>7596</v>
+        <v>7595</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>7445</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>7541</v>
+        <v>7540</v>
       </c>
       <c r="F16" s="37" t="s">
         <v>7485</v>
@@ -24167,19 +24170,19 @@
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="30" t="s">
-        <v>7601</v>
+        <v>7600</v>
       </c>
       <c r="B17" s="30" t="s">
         <v>52</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>7596</v>
+        <v>7595</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>7445</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>7542</v>
+        <v>7541</v>
       </c>
       <c r="F17" s="37" t="s">
         <v>7485</v>
@@ -24209,13 +24212,13 @@
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="30" t="s">
-        <v>7602</v>
+        <v>7601</v>
       </c>
       <c r="B18" s="30" t="s">
         <v>52</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>7596</v>
+        <v>7595</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>7445</v>
@@ -24251,25 +24254,25 @@
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="30" t="s">
-        <v>7603</v>
-      </c>
-      <c r="B19" s="30" t="s">
-        <v>52</v>
+        <v>7615</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1683</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>7596</v>
+        <v>7595</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>7445</v>
+        <v>7460</v>
       </c>
       <c r="E19" s="30" t="s">
-        <v>7533</v>
+        <v>7616</v>
       </c>
       <c r="F19" s="37" t="s">
-        <v>7485</v>
+        <v>39</v>
       </c>
       <c r="G19" s="36">
-        <v>120767</v>
+        <v>36527112</v>
       </c>
       <c r="H19" t="s">
         <v>7532</v>
@@ -24285,21 +24288,21 @@
       </c>
       <c r="L19" s="41">
         <f t="shared" ref="L19:L39" si="0">LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M19,CHAR(160)," ")," ",""))))</f>
-        <v>310</v>
+        <v>363</v>
       </c>
       <c r="M19" t="s">
-        <v>7537</v>
+        <v>7617</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="30" t="s">
-        <v>7604</v>
+        <v>7602</v>
       </c>
       <c r="B20" s="30" t="s">
         <v>52</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>7596</v>
+        <v>7595</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>7445</v>
@@ -24330,24 +24333,24 @@
         <v>310</v>
       </c>
       <c r="M20" t="s">
-        <v>7538</v>
+        <v>7537</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="30" t="s">
-        <v>7543</v>
+        <v>7542</v>
       </c>
       <c r="B21" t="s">
         <v>1683</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>7596</v>
+        <v>7595</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>7460</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>7592</v>
+        <v>7591</v>
       </c>
       <c r="F21" s="37" t="s">
         <v>7485</v>
@@ -24372,24 +24375,24 @@
         <v>886</v>
       </c>
       <c r="M21" t="s">
-        <v>7545</v>
+        <v>7544</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="30" t="s">
-        <v>7544</v>
+        <v>7543</v>
       </c>
       <c r="B22" t="s">
         <v>1683</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>7596</v>
+        <v>7595</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>7460</v>
       </c>
       <c r="E22" s="30" t="s">
-        <v>7591</v>
+        <v>7590</v>
       </c>
       <c r="F22" s="37" t="s">
         <v>7485</v>
@@ -24414,24 +24417,24 @@
         <v>910</v>
       </c>
       <c r="M22" t="s">
-        <v>7546</v>
+        <v>7545</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="30" t="s">
-        <v>7615</v>
+        <v>7613</v>
       </c>
       <c r="B23" t="s">
         <v>41</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>7596</v>
+        <v>7595</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>7445</v>
       </c>
       <c r="E23" s="30" t="s">
-        <v>7547</v>
+        <v>7546</v>
       </c>
       <c r="F23" s="37" t="s">
         <v>39</v>
@@ -24456,24 +24459,24 @@
         <v>351</v>
       </c>
       <c r="M23" t="s">
-        <v>7552</v>
+        <v>7551</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="30" t="s">
-        <v>7616</v>
+        <v>7614</v>
       </c>
       <c r="B24" t="s">
         <v>1728</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>7597</v>
+        <v>7596</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>7460</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>7548</v>
+        <v>7547</v>
       </c>
       <c r="F24" s="37" t="s">
         <v>39</v>
@@ -24498,24 +24501,24 @@
         <v>310</v>
       </c>
       <c r="M24" t="s">
-        <v>7549</v>
+        <v>7548</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="30" t="s">
-        <v>7609</v>
+        <v>7607</v>
       </c>
       <c r="B25" t="s">
         <v>41</v>
       </c>
       <c r="C25" s="30" t="s">
-        <v>7596</v>
+        <v>7595</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>7445</v>
       </c>
       <c r="E25" t="s">
-        <v>7547</v>
+        <v>7546</v>
       </c>
       <c r="F25" s="37" t="s">
         <v>39</v>
@@ -24540,24 +24543,24 @@
         <v>878</v>
       </c>
       <c r="M25" s="30" t="s">
-        <v>7581</v>
+        <v>7580</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="30" t="s">
-        <v>7610</v>
+        <v>7608</v>
       </c>
       <c r="B26" t="s">
         <v>41</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>7596</v>
+        <v>7595</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>7445</v>
       </c>
       <c r="E26" t="s">
-        <v>7547</v>
+        <v>7546</v>
       </c>
       <c r="F26" s="37" t="s">
         <v>39</v>
@@ -24582,24 +24585,24 @@
         <v>877</v>
       </c>
       <c r="M26" s="30" t="s">
-        <v>7582</v>
+        <v>7581</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="30" t="s">
-        <v>7611</v>
+        <v>7609</v>
       </c>
       <c r="B27" t="s">
         <v>41</v>
       </c>
       <c r="C27" s="30" t="s">
-        <v>7596</v>
+        <v>7595</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>7445</v>
       </c>
       <c r="E27" t="s">
-        <v>7547</v>
+        <v>7546</v>
       </c>
       <c r="F27" s="37" t="s">
         <v>39</v>
@@ -24624,24 +24627,24 @@
         <v>880</v>
       </c>
       <c r="M27" s="30" t="s">
-        <v>7583</v>
+        <v>7582</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="30" t="s">
-        <v>7612</v>
+        <v>7610</v>
       </c>
       <c r="B28" t="s">
         <v>41</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>7596</v>
+        <v>7595</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>7445</v>
       </c>
       <c r="E28" t="s">
-        <v>7547</v>
+        <v>7546</v>
       </c>
       <c r="F28" s="37" t="s">
         <v>39</v>
@@ -24666,24 +24669,24 @@
         <v>1085</v>
       </c>
       <c r="M28" s="30" t="s">
-        <v>7584</v>
+        <v>7583</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="30" t="s">
-        <v>7613</v>
+        <v>7611</v>
       </c>
       <c r="B29" t="s">
         <v>41</v>
       </c>
       <c r="C29" s="30" t="s">
-        <v>7596</v>
+        <v>7595</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>7445</v>
       </c>
       <c r="E29" t="s">
-        <v>7547</v>
+        <v>7546</v>
       </c>
       <c r="F29" s="37" t="s">
         <v>39</v>
@@ -24708,24 +24711,24 @@
         <v>877</v>
       </c>
       <c r="M29" s="30" t="s">
-        <v>7585</v>
+        <v>7584</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="30" t="s">
-        <v>7614</v>
+        <v>7612</v>
       </c>
       <c r="B30" t="s">
         <v>41</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>7596</v>
+        <v>7595</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>7445</v>
       </c>
       <c r="E30" t="s">
-        <v>7547</v>
+        <v>7546</v>
       </c>
       <c r="F30" s="37" t="s">
         <v>39</v>
@@ -24750,24 +24753,24 @@
         <v>1077</v>
       </c>
       <c r="M30" s="30" t="s">
-        <v>7586</v>
+        <v>7585</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="30" t="s">
-        <v>7550</v>
+        <v>7549</v>
       </c>
       <c r="B31" t="s">
         <v>47</v>
       </c>
       <c r="C31" s="30" t="s">
-        <v>7596</v>
+        <v>7595</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>48</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>7553</v>
+        <v>7552</v>
       </c>
       <c r="F31" s="37" t="s">
         <v>39</v>
@@ -24792,33 +24795,33 @@
         <v>1490</v>
       </c>
       <c r="M31" t="s">
-        <v>7551</v>
+        <v>7550</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="30" t="s">
-        <v>7556</v>
+        <v>7555</v>
       </c>
       <c r="B32" t="s">
         <v>47</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>7596</v>
+        <v>7595</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>48</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>7562</v>
+        <v>7561</v>
       </c>
       <c r="F32" s="37" t="s">
         <v>7469</v>
       </c>
       <c r="G32" s="36" t="s">
+        <v>7556</v>
+      </c>
+      <c r="H32" t="s">
         <v>7557</v>
-      </c>
-      <c r="H32" t="s">
-        <v>7558</v>
       </c>
       <c r="I32" t="s">
         <v>7419</v>
@@ -24834,33 +24837,33 @@
         <v>1709</v>
       </c>
       <c r="M32" s="30" t="s">
-        <v>7559</v>
+        <v>7558</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="30" t="s">
-        <v>7554</v>
+        <v>7553</v>
       </c>
       <c r="B33" t="s">
         <v>47</v>
       </c>
       <c r="C33" s="30" t="s">
-        <v>7596</v>
+        <v>7595</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>48</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>7563</v>
+        <v>7562</v>
       </c>
       <c r="F33" s="37" t="s">
         <v>7469</v>
       </c>
       <c r="G33" s="36" t="s">
+        <v>7556</v>
+      </c>
+      <c r="H33" t="s">
         <v>7557</v>
-      </c>
-      <c r="H33" t="s">
-        <v>7558</v>
       </c>
       <c r="I33" t="s">
         <v>7419</v>
@@ -24876,33 +24879,33 @@
         <v>1784</v>
       </c>
       <c r="M33" t="s">
-        <v>7560</v>
+        <v>7559</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="30" t="s">
-        <v>7555</v>
+        <v>7554</v>
       </c>
       <c r="B34" t="s">
         <v>47</v>
       </c>
       <c r="C34" s="30" t="s">
-        <v>7596</v>
+        <v>7595</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>48</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>7564</v>
+        <v>7563</v>
       </c>
       <c r="F34" s="37" t="s">
         <v>7469</v>
       </c>
       <c r="G34" s="36" t="s">
+        <v>7556</v>
+      </c>
+      <c r="H34" t="s">
         <v>7557</v>
-      </c>
-      <c r="H34" t="s">
-        <v>7558</v>
       </c>
       <c r="I34" t="s">
         <v>7419</v>
@@ -24918,24 +24921,24 @@
         <v>1223</v>
       </c>
       <c r="M34" s="30" t="s">
-        <v>7561</v>
+        <v>7560</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="30" t="s">
-        <v>7589</v>
+        <v>7588</v>
       </c>
       <c r="B35" t="s">
         <v>47</v>
       </c>
       <c r="C35" s="30" t="s">
-        <v>7596</v>
+        <v>7595</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>48</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>7593</v>
+        <v>7592</v>
       </c>
       <c r="F35" s="37" t="s">
         <v>39</v>
@@ -24960,36 +24963,36 @@
         <v>763</v>
       </c>
       <c r="M35" t="s">
-        <v>7590</v>
+        <v>7589</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="30" t="s">
-        <v>7565</v>
+        <v>7564</v>
       </c>
       <c r="B36" t="s">
         <v>1683</v>
       </c>
       <c r="C36" s="30" t="s">
-        <v>7598</v>
+        <v>7597</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>7460</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>7594</v>
+        <v>7593</v>
       </c>
       <c r="F36" s="37" t="s">
         <v>7529</v>
       </c>
       <c r="G36" s="42" t="s">
-        <v>7588</v>
+        <v>7587</v>
       </c>
       <c r="H36" t="s">
         <v>7417</v>
       </c>
       <c r="I36" t="s">
-        <v>7587</v>
+        <v>7586</v>
       </c>
       <c r="J36" t="b">
         <v>0</v>
@@ -25002,24 +25005,24 @@
         <v>310</v>
       </c>
       <c r="M36" t="s">
-        <v>7573</v>
+        <v>7572</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="30" t="s">
-        <v>7566</v>
+        <v>7565</v>
       </c>
       <c r="B37" t="s">
         <v>1683</v>
       </c>
       <c r="C37" s="30" t="s">
-        <v>7596</v>
+        <v>7595</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>7460</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>7595</v>
+        <v>7594</v>
       </c>
       <c r="F37" s="37" t="s">
         <v>39</v>
@@ -25031,7 +25034,7 @@
         <v>7417</v>
       </c>
       <c r="I37" t="s">
-        <v>7587</v>
+        <v>7586</v>
       </c>
       <c r="J37" t="b">
         <v>0</v>
@@ -25044,24 +25047,24 @@
         <v>397</v>
       </c>
       <c r="M37" t="s">
-        <v>7574</v>
+        <v>7573</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="30" t="s">
-        <v>7567</v>
+        <v>7566</v>
       </c>
       <c r="B38" t="s">
         <v>1683</v>
       </c>
       <c r="C38" s="30" t="s">
-        <v>7596</v>
+        <v>7595</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>7460</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>7595</v>
+        <v>7594</v>
       </c>
       <c r="F38" s="37" t="s">
         <v>39</v>
@@ -25073,7 +25076,7 @@
         <v>7417</v>
       </c>
       <c r="I38" t="s">
-        <v>7587</v>
+        <v>7586</v>
       </c>
       <c r="J38" t="b">
         <v>0</v>
@@ -25086,24 +25089,24 @@
         <v>406</v>
       </c>
       <c r="M38" s="30" t="s">
-        <v>7575</v>
+        <v>7574</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="30" t="s">
-        <v>7568</v>
+        <v>7567</v>
       </c>
       <c r="B39" t="s">
         <v>1683</v>
       </c>
       <c r="C39" s="30" t="s">
-        <v>7596</v>
+        <v>7595</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>7460</v>
       </c>
       <c r="E39" s="30" t="s">
-        <v>7595</v>
+        <v>7594</v>
       </c>
       <c r="F39" s="37" t="s">
         <v>39</v>
@@ -25115,7 +25118,7 @@
         <v>7417</v>
       </c>
       <c r="I39" t="s">
-        <v>7587</v>
+        <v>7586</v>
       </c>
       <c r="J39" t="b">
         <v>0</v>
@@ -25128,24 +25131,24 @@
         <v>310</v>
       </c>
       <c r="M39" s="30" t="s">
-        <v>7576</v>
+        <v>7575</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="30" t="s">
-        <v>7569</v>
+        <v>7568</v>
       </c>
       <c r="B40" t="s">
         <v>1683</v>
       </c>
       <c r="C40" s="30" t="s">
-        <v>7596</v>
+        <v>7595</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>7460</v>
       </c>
       <c r="E40" s="30" t="s">
-        <v>7595</v>
+        <v>7594</v>
       </c>
       <c r="F40" s="37" t="s">
         <v>39</v>
@@ -25157,7 +25160,7 @@
         <v>7417</v>
       </c>
       <c r="I40" t="s">
-        <v>7587</v>
+        <v>7586</v>
       </c>
       <c r="J40" t="b">
         <v>0</v>
@@ -25170,24 +25173,24 @@
         <v>310</v>
       </c>
       <c r="M40" s="30" t="s">
-        <v>7577</v>
+        <v>7576</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="30" t="s">
-        <v>7570</v>
+        <v>7569</v>
       </c>
       <c r="B41" t="s">
         <v>1683</v>
       </c>
       <c r="C41" s="30" t="s">
-        <v>7596</v>
+        <v>7595</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>7460</v>
       </c>
       <c r="E41" s="30" t="s">
-        <v>7595</v>
+        <v>7594</v>
       </c>
       <c r="F41" s="37" t="s">
         <v>39</v>
@@ -25199,7 +25202,7 @@
         <v>7417</v>
       </c>
       <c r="I41" t="s">
-        <v>7587</v>
+        <v>7586</v>
       </c>
       <c r="J41" t="b">
         <v>0</v>
@@ -25212,24 +25215,24 @@
         <v>313</v>
       </c>
       <c r="M41" s="30" t="s">
-        <v>7578</v>
+        <v>7577</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="30" t="s">
-        <v>7571</v>
+        <v>7570</v>
       </c>
       <c r="B42" t="s">
         <v>1683</v>
       </c>
       <c r="C42" s="30" t="s">
-        <v>7596</v>
+        <v>7595</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>7460</v>
       </c>
       <c r="E42" s="30" t="s">
-        <v>7595</v>
+        <v>7594</v>
       </c>
       <c r="F42" s="37" t="s">
         <v>39</v>
@@ -25241,7 +25244,7 @@
         <v>7417</v>
       </c>
       <c r="I42" t="s">
-        <v>7587</v>
+        <v>7586</v>
       </c>
       <c r="J42" t="b">
         <v>0</v>
@@ -25254,24 +25257,24 @@
         <v>310</v>
       </c>
       <c r="M42" s="30" t="s">
-        <v>7579</v>
+        <v>7578</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="30" t="s">
-        <v>7572</v>
+        <v>7571</v>
       </c>
       <c r="B43" t="s">
         <v>1683</v>
       </c>
       <c r="C43" s="30" t="s">
-        <v>7596</v>
+        <v>7595</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>7460</v>
       </c>
       <c r="E43" s="30" t="s">
-        <v>7595</v>
+        <v>7594</v>
       </c>
       <c r="F43" s="37" t="s">
         <v>39</v>
@@ -25283,7 +25286,7 @@
         <v>7417</v>
       </c>
       <c r="I43" t="s">
-        <v>7587</v>
+        <v>7586</v>
       </c>
       <c r="J43" t="b">
         <v>0</v>
@@ -25296,24 +25299,24 @@
         <v>327</v>
       </c>
       <c r="M43" s="30" t="s">
-        <v>7580</v>
+        <v>7579</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>7605</v>
+        <v>7603</v>
       </c>
       <c r="B44" t="s">
         <v>1683</v>
       </c>
       <c r="C44" s="30" t="s">
-        <v>7596</v>
+        <v>7595</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>7460</v>
       </c>
       <c r="E44" s="30" t="s">
-        <v>7606</v>
+        <v>7604</v>
       </c>
       <c r="F44" s="37" t="s">
         <v>39</v>
@@ -25338,7 +25341,7 @@
         <v>310</v>
       </c>
       <c r="M44" s="30" t="s">
-        <v>7607</v>
+        <v>7605</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -26603,7 +26606,7 @@
           <x14:formula1>
             <xm:f>'Ontology Terms'!$B$2:$B$2518</xm:f>
           </x14:formula1>
-          <xm:sqref>B15:B44 B59:B68</xm:sqref>
+          <xm:sqref>B59:B68 B15:B44</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
@@ -61938,12 +61941,12 @@
     </row>
     <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>7558</v>
+        <v>7557</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>7587</v>
+        <v>7586</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>